<commit_message>
refactoring scripts, updating files, adding 'real_time' ratioo to summary spreadsheets and saving as csv files; need to work on formatting.
</commit_message>
<xml_diff>
--- a/summary_spreadsheets/multinode_benchmark_results_summary.xlsx
+++ b/summary_spreadsheets/multinode_benchmark_results_summary.xlsx
@@ -19,7 +19,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="22">
+  <si>
+    <t>elapsed_time_ratio</t>
+  </si>
   <si>
     <t>spf_ratio</t>
   </si>
@@ -439,233 +442,296 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D3">
         <v>414.2393639987217</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3">
+        <v>414.2393639987217</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D4">
         <v>1.028231177573642</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4">
+        <v>1.028231177573642</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D5">
         <v>3.512383880644123</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5">
+        <v>3.512383880644123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D6">
         <v>1.431276638478164</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6">
+        <v>1.431276638478164</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="1"/>
       <c r="B7" s="1">
         <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D8">
         <v>2.204123275762006</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8">
+        <v>2.204123275762006</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D9">
         <v>0.01118168061816597</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E9">
+        <v>0.01118168061816597</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D10">
         <v>0.009739092708668433</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="E10">
+        <v>0.009739092708668433</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D11">
         <v>0.009385503273635349</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11">
+        <v>0.009385503273635349</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="1"/>
       <c r="B12" s="1">
         <v>4</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D13">
         <v>120.6311428616924</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="E13">
+        <v>120.6311428616924</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D14">
         <v>1.005046860188864</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="E14">
+        <v>1.005046860188864</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D15">
         <v>0.6479166653796352</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="E15">
+        <v>0.6479166653796352</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D16">
         <v>0.6456940956112384</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16">
+        <v>0.6456940956112384</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="1"/>
       <c r="B17" s="1">
         <v>8</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D18">
         <v>23.12031455957467</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18">
+        <v>23.12031455957467</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D19">
         <v>0.3336097501135856</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="E19">
+        <v>0.3336097501135856</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D20">
         <v>0.1867451589563411</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="E20">
+        <v>0.1867451589563411</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D21">
+        <v>0.1819662395244153</v>
+      </c>
+      <c r="E21">
         <v>0.1819662395244153</v>
       </c>
     </row>
@@ -683,233 +749,296 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D3">
         <v>330.7004734175064</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3">
+        <v>330.7004734175064</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D4">
         <v>1.181978885850061</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4">
+        <v>1.181978885850061</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D5">
         <v>1.208333321902606</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5">
+        <v>1.208333321902606</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D6">
         <v>1.266961825925632</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6">
+        <v>1.266961825925632</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="1"/>
       <c r="B7" s="1">
         <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D8">
         <v>231.9685252702395</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8">
+        <v>231.9685252702395</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D9">
         <v>1.093423995111745</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E9">
+        <v>1.093423995111745</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D10">
         <v>1.043289373814342</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="E10">
+        <v>1.043289373814342</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D11">
         <v>0.9435295198866849</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11">
+        <v>0.9435295198866849</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="1"/>
       <c r="B12" s="1">
         <v>4</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D13">
         <v>192.9435269470882</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="E13">
+        <v>192.9435269470882</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D14">
         <v>1.610578780168383</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="E14">
+        <v>1.610578780168383</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D15">
         <v>1.007666280221873</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="E15">
+        <v>1.007666280221873</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D16">
         <v>1.120033271682305</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16">
+        <v>1.120033271682305</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="1"/>
       <c r="B17" s="1">
         <v>8</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D18">
         <v>100.6712253676607</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18">
+        <v>100.6712253676607</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D19">
         <v>1.780722679881865</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="E19">
+        <v>1.780722679881865</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D20">
         <v>0.9281915809706429</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="E20">
+        <v>0.9281915809706429</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D21">
+        <v>0.886690641558511</v>
+      </c>
+      <c r="E21">
         <v>0.886690641558511</v>
       </c>
     </row>
@@ -927,233 +1056,296 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D3">
         <v>0.9435639823523477</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3">
+        <v>0.9435639823523477</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D4">
         <v>1.060121470154189</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4">
+        <v>1.060121470154189</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D5">
         <v>1.064675410041091</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5">
+        <v>1.064675410041091</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D6">
         <v>0.9682819863115475</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6">
+        <v>0.9682819863115475</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="1"/>
       <c r="B7" s="1">
         <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D8">
         <v>225.9668285269331</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8">
+        <v>225.9668285269331</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D9">
         <v>0.9090417806642039</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E9">
+        <v>0.9090417806642039</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D10">
         <v>4.72454827484734</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="E10">
+        <v>4.72454827484734</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D11">
         <v>4.678394481572738</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11">
+        <v>4.678394481572738</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="1"/>
       <c r="B12" s="1">
         <v>4</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D13">
         <v>157.879355478262</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="E13">
+        <v>157.879355478262</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D14">
         <v>0.6731253732532476</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="E14">
+        <v>0.6731253732532476</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D15">
         <v>3.665070623150748</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="E15">
+        <v>3.665070623150748</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D16">
         <v>2.938145464950471</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16">
+        <v>2.938145464950471</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="1"/>
       <c r="B17" s="1">
         <v>8</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D18">
         <v>105.2195177464722</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18">
+        <v>105.2195177464722</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D19">
         <v>0.7007826888548608</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="E19">
+        <v>0.7007826888548608</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D20">
         <v>1.806874346148886</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="E20">
+        <v>1.806874346148886</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D21">
+        <v>1.876405585252029</v>
+      </c>
+      <c r="E21">
         <v>1.876405585252029</v>
       </c>
     </row>
@@ -1171,233 +1363,296 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D3">
         <v>0.9435639823523477</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3">
+        <v>0.9435639823523477</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D4">
         <v>1.060121470154189</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4">
+        <v>1.060121470154189</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D5">
         <v>1.064675410041091</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5">
+        <v>1.064675410041091</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D6">
         <v>0.9682819863115475</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6">
+        <v>0.9682819863115475</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="1"/>
       <c r="B7" s="1">
         <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D8">
         <v>225.9668285269331</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8">
+        <v>225.9668285269331</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D9">
         <v>0.9090417806642039</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E9">
+        <v>0.9090417806642039</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D10">
         <v>4.72454827484734</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="E10">
+        <v>4.72454827484734</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D11">
         <v>4.678394481572738</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11">
+        <v>4.678394481572738</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="1"/>
       <c r="B12" s="1">
         <v>4</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D13">
         <v>157.879355478262</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="E13">
+        <v>157.879355478262</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D14">
         <v>0.6731253732532476</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="E14">
+        <v>0.6731253732532476</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D15">
         <v>3.665070623150748</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="E15">
+        <v>3.665070623150748</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D16">
         <v>2.938145464950471</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16">
+        <v>2.938145464950471</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="1"/>
       <c r="B17" s="1">
         <v>8</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D18">
         <v>105.2195177464722</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18">
+        <v>105.2195177464722</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D19">
         <v>0.7007826888548608</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="E19">
+        <v>0.7007826888548608</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D20">
         <v>1.806874346148886</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="E20">
+        <v>1.806874346148886</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D21">
+        <v>1.876405585252029</v>
+      </c>
+      <c r="E21">
         <v>1.876405585252029</v>
       </c>
     </row>
@@ -1415,44 +1670,47 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+        <v>15</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1466,12 +1724,15 @@
       <c r="G2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="H2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D3">
         <v>1.631098005983478</v>
@@ -1485,12 +1746,15 @@
       <c r="G3">
         <v>1.277144473418524</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="H3">
+        <v>1.277144473418524</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D4">
         <v>1.606472437362901</v>
@@ -1504,12 +1768,15 @@
       <c r="G4">
         <v>1.267466937384523</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="H4">
+        <v>1.267466937384523</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D5">
         <v>1.585843969335239</v>
@@ -1523,12 +1790,15 @@
       <c r="G5">
         <v>1.259302969636473</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="H5">
+        <v>1.259302969636473</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D6">
         <v>1.872859726645483</v>
@@ -1542,14 +1812,17 @@
       <c r="G6">
         <v>1.368524653283777</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="H6">
+        <v>1.368524653283777</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="1"/>
       <c r="B7" s="1">
         <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -1563,12 +1836,15 @@
       <c r="G7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="H7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D8">
         <v>40219.51109919947</v>
@@ -1582,12 +1858,15 @@
       <c r="G8">
         <v>200.54802690065</v>
       </c>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="H8">
+        <v>200.54802690065</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D9">
         <v>0.8931655725849961</v>
@@ -1601,12 +1880,15 @@
       <c r="G9">
         <v>0.9450743738791469</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="H9">
+        <v>0.9450743738791469</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D10">
         <v>1.632792625499382</v>
@@ -1620,12 +1902,15 @@
       <c r="G10">
         <v>1.277807740372132</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="H10">
+        <v>1.277807740372132</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D11">
         <v>1.598918413577855</v>
@@ -1634,19 +1919,22 @@
         <v>1.598918413577855</v>
       </c>
       <c r="F11">
+        <v>1.264483456074377</v>
+      </c>
+      <c r="G11">
         <v>1.264483456074378</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>1.264483456074377</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:8">
       <c r="A12" s="1"/>
       <c r="B12" s="1">
         <v>4</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -1660,12 +1948,15 @@
       <c r="G12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="H12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D13">
         <v>16683.52383416874</v>
@@ -1679,12 +1970,15 @@
       <c r="G13">
         <v>129.1647156639779</v>
       </c>
-    </row>
-    <row r="14" spans="1:7">
+      <c r="H13">
+        <v>129.1647156639779</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D14">
         <v>1.514401343519805</v>
@@ -1693,17 +1987,20 @@
         <v>1.514401343519806</v>
       </c>
       <c r="F14">
+        <v>1.230610149112736</v>
+      </c>
+      <c r="G14">
         <v>1.230610149112735</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>1.230610149112736</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:8">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D15">
         <v>2.071497716208372</v>
@@ -1717,12 +2014,15 @@
       <c r="G15">
         <v>1.439269853087512</v>
       </c>
-    </row>
-    <row r="16" spans="1:7">
+      <c r="H15">
+        <v>1.439269853087512</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D16">
         <v>2.88904402681033</v>
@@ -1736,14 +2036,17 @@
       <c r="G16">
         <v>1.699718805686186</v>
       </c>
-    </row>
-    <row r="17" spans="1:7">
+      <c r="H16">
+        <v>1.699718805686186</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" s="1"/>
       <c r="B17" s="1">
         <v>8</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -1757,12 +2060,15 @@
       <c r="G17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:7">
+      <c r="H17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D18">
         <v>6040.81103932062</v>
@@ -1776,12 +2082,15 @@
       <c r="G18">
         <v>77.72265457582611</v>
       </c>
-    </row>
-    <row r="19" spans="1:7">
+      <c r="H18">
+        <v>77.72265457582611</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D19">
         <v>2.226879116634304</v>
@@ -1795,12 +2104,15 @@
       <c r="G19">
         <v>1.492273136425073</v>
       </c>
-    </row>
-    <row r="20" spans="1:7">
+      <c r="H19">
+        <v>1.492273136425073</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D20">
         <v>2.207722524362522</v>
@@ -1814,12 +2126,15 @@
       <c r="G20">
         <v>1.485840678563465</v>
       </c>
-    </row>
-    <row r="21" spans="1:7">
+      <c r="H20">
+        <v>1.485840678563465</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D21">
         <v>2.516055352821687</v>
@@ -1831,6 +2146,9 @@
         <v>1.586207851736727</v>
       </c>
       <c r="G21">
+        <v>1.586207851736727</v>
+      </c>
+      <c r="H21">
         <v>1.586207851736727</v>
       </c>
     </row>
@@ -1848,35 +2166,38 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F120"/>
+  <dimension ref="A1:G120"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -1885,7 +2206,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -1893,13 +2214,16 @@
       <c r="F2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E3">
         <v>89.78283223674258</v>
@@ -1907,13 +2231,16 @@
       <c r="F3">
         <v>89.78283223674258</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3">
+        <v>89.78283223674258</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E4">
         <v>0.8956669600910819</v>
@@ -1921,13 +2248,16 @@
       <c r="F4">
         <v>0.8956669600910819</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4">
+        <v>0.8956669600910819</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E5">
         <v>1.622970409389778</v>
@@ -1935,13 +2265,16 @@
       <c r="F5">
         <v>1.622970409389778</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5">
+        <v>1.622970409389778</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E6">
         <v>1.077075559615454</v>
@@ -1949,15 +2282,18 @@
       <c r="F6">
         <v>1.077075559615454</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6">
+        <v>1.077075559615454</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1">
         <v>4</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -1965,13 +2301,16 @@
       <c r="F7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E8">
         <v>72.83303589992376</v>
@@ -1979,13 +2318,16 @@
       <c r="F8">
         <v>72.83303589992376</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8">
+        <v>72.83303589992376</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E9">
         <v>0.8061104475056362</v>
@@ -1993,13 +2335,16 @@
       <c r="F9">
         <v>0.8061104475056362</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="G9">
+        <v>0.8061104475056362</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E10">
         <v>1.758517619744551</v>
@@ -2007,13 +2352,16 @@
       <c r="F10">
         <v>1.758517619744551</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="G10">
+        <v>1.758517619744551</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E11">
         <v>1.168943875283844</v>
@@ -2021,15 +2369,18 @@
       <c r="F11">
         <v>1.168943875283844</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="G11">
+        <v>1.168943875283844</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1">
         <v>16</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -2037,13 +2388,16 @@
       <c r="F12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="G12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E13">
         <v>67.78463935489476</v>
@@ -2051,13 +2405,16 @@
       <c r="F13">
         <v>67.78463935489476</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="G13">
+        <v>67.78463935489476</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E14">
         <v>2.105372452874108</v>
@@ -2065,13 +2422,16 @@
       <c r="F14">
         <v>2.105372452874108</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="G14">
+        <v>2.105372452874108</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E15">
         <v>1.403689640909411</v>
@@ -2079,13 +2439,16 @@
       <c r="F15">
         <v>1.403689640909411</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="G15">
+        <v>1.403689640909411</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E16">
         <v>1.210800912055891</v>
@@ -2093,15 +2456,18 @@
       <c r="F16">
         <v>1.210800912055891</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="G16">
+        <v>1.210800912055891</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1">
         <v>64</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -2109,13 +2475,16 @@
       <c r="F17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="G17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E18">
         <v>1.68241024430724</v>
@@ -2123,13 +2492,16 @@
       <c r="F18">
         <v>1.68241024430724</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="G18">
+        <v>1.68241024430724</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E19">
         <v>0.1175856896847261</v>
@@ -2137,13 +2509,16 @@
       <c r="F19">
         <v>0.1175856896847261</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="G19">
+        <v>0.1175856896847261</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E20">
         <v>0.04761894651535323</v>
@@ -2151,13 +2526,16 @@
       <c r="F20">
         <v>0.04761894651535323</v>
       </c>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="G20">
+        <v>0.04761894651535323</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E21">
         <v>0.06243857028336713</v>
@@ -2165,8 +2543,11 @@
       <c r="F21">
         <v>0.06243857028336713</v>
       </c>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="G21">
+        <v>0.06243857028336713</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" s="1"/>
       <c r="B22" s="1">
         <v>16</v>
@@ -2175,7 +2556,7 @@
         <v>1</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E22">
         <v>1</v>
@@ -2183,13 +2564,16 @@
       <c r="F22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="G22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E23">
         <v>114.3223466482583</v>
@@ -2197,13 +2581,16 @@
       <c r="F23">
         <v>114.3223466482583</v>
       </c>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="G23">
+        <v>114.3223466482583</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E24">
         <v>1.086597113351394</v>
@@ -2211,13 +2598,16 @@
       <c r="F24">
         <v>1.086597113351394</v>
       </c>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="G24">
+        <v>1.086597113351394</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E25">
         <v>1.629422956345736</v>
@@ -2225,13 +2615,16 @@
       <c r="F25">
         <v>1.629422956345736</v>
       </c>
-    </row>
-    <row r="26" spans="1:6">
+      <c r="G25">
+        <v>1.629422956345736</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E26">
         <v>1.643552780968021</v>
@@ -2239,15 +2632,18 @@
       <c r="F26">
         <v>1.643552780968021</v>
       </c>
-    </row>
-    <row r="27" spans="1:6">
+      <c r="G26">
+        <v>1.643552780968021</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1">
         <v>4</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E27">
         <v>1</v>
@@ -2255,13 +2651,16 @@
       <c r="F27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:6">
+      <c r="G27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E28">
         <v>86.55085846678699</v>
@@ -2269,13 +2668,16 @@
       <c r="F28">
         <v>86.55085846678699</v>
       </c>
-    </row>
-    <row r="29" spans="1:6">
+      <c r="G28">
+        <v>86.55085846678699</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E29">
         <v>1.174927066192191</v>
@@ -2283,13 +2685,16 @@
       <c r="F29">
         <v>1.174927066192191</v>
       </c>
-    </row>
-    <row r="30" spans="1:6">
+      <c r="G29">
+        <v>1.174927066192191</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E30">
         <v>1.18583941631698</v>
@@ -2297,13 +2702,16 @@
       <c r="F30">
         <v>1.18583941631698</v>
       </c>
-    </row>
-    <row r="31" spans="1:6">
+      <c r="G30">
+        <v>1.18583941631698</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E31">
         <v>1.343238987305001</v>
@@ -2311,15 +2719,18 @@
       <c r="F31">
         <v>1.343238987305001</v>
       </c>
-    </row>
-    <row r="32" spans="1:6">
+      <c r="G31">
+        <v>1.343238987305001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1">
         <v>16</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E32">
         <v>1</v>
@@ -2327,13 +2738,16 @@
       <c r="F32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:6">
+      <c r="G32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E33">
         <v>44.87243578827441</v>
@@ -2341,13 +2755,16 @@
       <c r="F33">
         <v>44.87243578827441</v>
       </c>
-    </row>
-    <row r="34" spans="1:6">
+      <c r="G33">
+        <v>44.87243578827441</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E34">
         <v>1.825954736924908</v>
@@ -2355,13 +2772,16 @@
       <c r="F34">
         <v>1.825954736924908</v>
       </c>
-    </row>
-    <row r="35" spans="1:6">
+      <c r="G34">
+        <v>1.825954736924908</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E35">
         <v>1.07059832111179</v>
@@ -2369,13 +2789,16 @@
       <c r="F35">
         <v>1.07059832111179</v>
       </c>
-    </row>
-    <row r="36" spans="1:6">
+      <c r="G35">
+        <v>1.07059832111179</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E36">
         <v>1.058936781932113</v>
@@ -2383,15 +2806,18 @@
       <c r="F36">
         <v>1.058936781932113</v>
       </c>
-    </row>
-    <row r="37" spans="1:6">
+      <c r="G36">
+        <v>1.058936781932113</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1">
         <v>64</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E37">
         <v>1</v>
@@ -2399,13 +2825,16 @@
       <c r="F37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:6">
+      <c r="G37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E38">
         <v>8.138883559388573</v>
@@ -2413,13 +2842,16 @@
       <c r="F38">
         <v>8.138883559388573</v>
       </c>
-    </row>
-    <row r="39" spans="1:6">
+      <c r="G38">
+        <v>8.138883559388573</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E39">
         <v>0.5189524484568723</v>
@@ -2427,13 +2859,16 @@
       <c r="F39">
         <v>0.5189524484568723</v>
       </c>
-    </row>
-    <row r="40" spans="1:6">
+      <c r="G39">
+        <v>0.5189524484568723</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E40">
         <v>0.2862537280118536</v>
@@ -2441,13 +2876,16 @@
       <c r="F40">
         <v>0.2862537280118536</v>
       </c>
-    </row>
-    <row r="41" spans="1:6">
+      <c r="G40">
+        <v>0.2862537280118536</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E41">
         <v>0.2181377076922102</v>
@@ -2455,8 +2893,11 @@
       <c r="F41">
         <v>0.2181377076922102</v>
       </c>
-    </row>
-    <row r="42" spans="1:6">
+      <c r="G41">
+        <v>0.2181377076922102</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42" s="1"/>
       <c r="B42" s="1">
         <v>64</v>
@@ -2465,7 +2906,7 @@
         <v>1</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E42">
         <v>1</v>
@@ -2473,13 +2914,16 @@
       <c r="F42">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:6">
+      <c r="G42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E43">
         <v>85.94391614769603</v>
@@ -2487,13 +2931,16 @@
       <c r="F43">
         <v>85.94391614769603</v>
       </c>
-    </row>
-    <row r="44" spans="1:6">
+      <c r="G43">
+        <v>85.94391614769603</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E44">
         <v>0.9024757401942765</v>
@@ -2501,13 +2948,16 @@
       <c r="F44">
         <v>0.9024757401942765</v>
       </c>
-    </row>
-    <row r="45" spans="1:6">
+      <c r="G44">
+        <v>0.9024757401942765</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E45">
         <v>2.173957727847946</v>
@@ -2515,13 +2965,16 @@
       <c r="F45">
         <v>2.173957727847946</v>
       </c>
-    </row>
-    <row r="46" spans="1:6">
+      <c r="G45">
+        <v>2.173957727847946</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E46">
         <v>1.106434292357325</v>
@@ -2529,15 +2982,18 @@
       <c r="F46">
         <v>1.106434292357325</v>
       </c>
-    </row>
-    <row r="47" spans="1:6">
+      <c r="G46">
+        <v>1.106434292357325</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1">
         <v>4</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E47">
         <v>1</v>
@@ -2545,13 +3001,16 @@
       <c r="F47">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:6">
+      <c r="G47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E48">
         <v>89.60482592352977</v>
@@ -2559,13 +3018,16 @@
       <c r="F48">
         <v>89.60482592352977</v>
       </c>
-    </row>
-    <row r="49" spans="1:6">
+      <c r="G48">
+        <v>89.60482592352977</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E49">
         <v>1.134727682010267</v>
@@ -2573,13 +3035,16 @@
       <c r="F49">
         <v>1.134727682010267</v>
       </c>
-    </row>
-    <row r="50" spans="1:6">
+      <c r="G49">
+        <v>1.134727682010267</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E50">
         <v>2.242870346956074</v>
@@ -2587,13 +3052,16 @@
       <c r="F50">
         <v>2.242870346956074</v>
       </c>
-    </row>
-    <row r="51" spans="1:6">
+      <c r="G50">
+        <v>2.242870346956074</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E51">
         <v>1.308329054902935</v>
@@ -2601,15 +3069,18 @@
       <c r="F51">
         <v>1.308329054902935</v>
       </c>
-    </row>
-    <row r="52" spans="1:6">
+      <c r="G51">
+        <v>1.308329054902935</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1">
         <v>16</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E52">
         <v>1</v>
@@ -2617,13 +3088,16 @@
       <c r="F52">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:6">
+      <c r="G52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E53">
         <v>5.572712231505021</v>
@@ -2631,13 +3105,16 @@
       <c r="F53">
         <v>5.572712231505021</v>
       </c>
-    </row>
-    <row r="54" spans="1:6">
+      <c r="G53">
+        <v>5.572712231505021</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E54">
         <v>0.1813001785820309</v>
@@ -2645,13 +3122,16 @@
       <c r="F54">
         <v>0.1813001785820309</v>
       </c>
-    </row>
-    <row r="55" spans="1:6">
+      <c r="G54">
+        <v>0.1813001785820309</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E55">
         <v>0.1232298263498409</v>
@@ -2659,13 +3139,16 @@
       <c r="F55">
         <v>0.1232298263498409</v>
       </c>
-    </row>
-    <row r="56" spans="1:6">
+      <c r="G55">
+        <v>0.1232298263498409</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E56">
         <v>0.1078411098594783</v>
@@ -2673,15 +3156,18 @@
       <c r="F56">
         <v>0.1078411098594783</v>
       </c>
-    </row>
-    <row r="57" spans="1:6">
+      <c r="G56">
+        <v>0.1078411098594783</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1">
         <v>64</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E57">
         <v>1</v>
@@ -2689,13 +3175,16 @@
       <c r="F57">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:6">
+      <c r="G57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E58">
         <v>1.541367934253603</v>
@@ -2703,13 +3192,16 @@
       <c r="F58">
         <v>1.541367934253603</v>
       </c>
-    </row>
-    <row r="59" spans="1:6">
+      <c r="G58">
+        <v>1.541367934253603</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E59">
         <v>0.07219760225253845</v>
@@ -2717,13 +3209,16 @@
       <c r="F59">
         <v>0.07219760225253845</v>
       </c>
-    </row>
-    <row r="60" spans="1:6">
+      <c r="G59">
+        <v>0.07219760225253845</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E60">
         <v>0.03175142187081256</v>
@@ -2731,13 +3226,16 @@
       <c r="F60">
         <v>0.03175142187081256</v>
       </c>
-    </row>
-    <row r="61" spans="1:6">
+      <c r="G60">
+        <v>0.03175142187081256</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E61">
         <v>0.03635015449343772</v>
@@ -2745,8 +3243,11 @@
       <c r="F61">
         <v>0.03635015449343772</v>
       </c>
-    </row>
-    <row r="62" spans="1:6">
+      <c r="G61">
+        <v>0.03635015449343772</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
       <c r="A62" s="1"/>
       <c r="B62" s="1">
         <v>256</v>
@@ -2755,7 +3256,7 @@
         <v>1</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E62">
         <v>1</v>
@@ -2763,13 +3264,16 @@
       <c r="F62">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:6">
+      <c r="G62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E63">
         <v>87.58442267979227</v>
@@ -2777,13 +3281,16 @@
       <c r="F63">
         <v>87.58442267979227</v>
       </c>
-    </row>
-    <row r="64" spans="1:6">
+      <c r="G63">
+        <v>87.58442267979227</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E64">
         <v>0.8268447523765605</v>
@@ -2791,13 +3298,16 @@
       <c r="F64">
         <v>0.8268447523765605</v>
       </c>
-    </row>
-    <row r="65" spans="1:6">
+      <c r="G64">
+        <v>0.8268447523765605</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E65">
         <v>1.704276806658666</v>
@@ -2805,13 +3315,16 @@
       <c r="F65">
         <v>1.704276806658666</v>
       </c>
-    </row>
-    <row r="66" spans="1:6">
+      <c r="G65">
+        <v>1.704276806658666</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E66">
         <v>1.596775567897026</v>
@@ -2819,15 +3332,18 @@
       <c r="F66">
         <v>1.596775567897026</v>
       </c>
-    </row>
-    <row r="67" spans="1:6">
+      <c r="G66">
+        <v>1.596775567897026</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1">
         <v>4</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E67">
         <v>1</v>
@@ -2835,13 +3351,16 @@
       <c r="F67">
         <v>1</v>
       </c>
-    </row>
-    <row r="68" spans="1:6">
+      <c r="G67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E68">
         <v>69.57884361774389</v>
@@ -2849,13 +3368,16 @@
       <c r="F68">
         <v>69.57884361774389</v>
       </c>
-    </row>
-    <row r="69" spans="1:6">
+      <c r="G68">
+        <v>69.57884361774389</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E69">
         <v>1.339947959663514</v>
@@ -2863,13 +3385,16 @@
       <c r="F69">
         <v>1.339947959663514</v>
       </c>
-    </row>
-    <row r="70" spans="1:6">
+      <c r="G69">
+        <v>1.339947959663514</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E70">
         <v>2.760403364857098</v>
@@ -2877,13 +3402,16 @@
       <c r="F70">
         <v>2.760403364857098</v>
       </c>
-    </row>
-    <row r="71" spans="1:6">
+      <c r="G70">
+        <v>2.760403364857098</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
       <c r="D71" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E71">
         <v>1.623740007314907</v>
@@ -2891,15 +3419,18 @@
       <c r="F71">
         <v>1.623740007314907</v>
       </c>
-    </row>
-    <row r="72" spans="1:6">
+      <c r="G71">
+        <v>1.623740007314907</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1">
         <v>16</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E72">
         <v>1</v>
@@ -2907,13 +3438,16 @@
       <c r="F72">
         <v>1</v>
       </c>
-    </row>
-    <row r="73" spans="1:6">
+      <c r="G72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E73">
         <v>0.8590609387652602</v>
@@ -2921,13 +3455,16 @@
       <c r="F73">
         <v>0.8590609387652602</v>
       </c>
-    </row>
-    <row r="74" spans="1:6">
+      <c r="G73">
+        <v>0.8590609387652602</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E74">
         <v>0.03445966757525627</v>
@@ -2935,13 +3472,16 @@
       <c r="F74">
         <v>0.03445966757525627</v>
       </c>
-    </row>
-    <row r="75" spans="1:6">
+      <c r="G74">
+        <v>0.03445966757525627</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E75">
         <v>0.02408804393152452</v>
@@ -2949,13 +3489,16 @@
       <c r="F75">
         <v>0.02408804393152452</v>
       </c>
-    </row>
-    <row r="76" spans="1:6">
+      <c r="G75">
+        <v>0.02408804393152452</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E76">
         <v>0.02427279304817658</v>
@@ -2963,15 +3506,18 @@
       <c r="F76">
         <v>0.02427279304817658</v>
       </c>
-    </row>
-    <row r="77" spans="1:6">
+      <c r="G76">
+        <v>0.02427279304817658</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1">
         <v>64</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E77">
         <v>1</v>
@@ -2979,13 +3525,16 @@
       <c r="F77">
         <v>1</v>
       </c>
-    </row>
-    <row r="78" spans="1:6">
+      <c r="G77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
       <c r="D78" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E78">
         <v>1.185151496758129</v>
@@ -2993,13 +3542,16 @@
       <c r="F78">
         <v>1.185151496758129</v>
       </c>
-    </row>
-    <row r="79" spans="1:6">
+      <c r="G78">
+        <v>1.185151496758129</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
       <c r="D79" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E79">
         <v>0.05958268897826299</v>
@@ -3007,13 +3559,16 @@
       <c r="F79">
         <v>0.05958268897826299</v>
       </c>
-    </row>
-    <row r="80" spans="1:6">
+      <c r="G79">
+        <v>0.05958268897826299</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E80">
         <v>0.02939762386920262</v>
@@ -3021,13 +3576,16 @@
       <c r="F80">
         <v>0.02939762386920262</v>
       </c>
-    </row>
-    <row r="81" spans="1:6">
+      <c r="G80">
+        <v>0.02939762386920262</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
       <c r="D81" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E81">
         <v>0.03027232211131487</v>
@@ -3035,8 +3593,11 @@
       <c r="F81">
         <v>0.03027232211131487</v>
       </c>
-    </row>
-    <row r="82" spans="1:6">
+      <c r="G81">
+        <v>0.03027232211131487</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
       <c r="A82" s="1"/>
       <c r="B82" s="1">
         <v>1024</v>
@@ -3045,7 +3606,7 @@
         <v>1</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E82">
         <v>1</v>
@@ -3053,13 +3614,16 @@
       <c r="F82">
         <v>1</v>
       </c>
-    </row>
-    <row r="83" spans="1:6">
+      <c r="G82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
       <c r="D83" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E83">
         <v>2.468957735378221</v>
@@ -3067,13 +3631,16 @@
       <c r="F83">
         <v>2.468957735378221</v>
       </c>
-    </row>
-    <row r="84" spans="1:6">
+      <c r="G83">
+        <v>2.468957735378221</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
       <c r="D84" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E84">
         <v>0.03244746077034172</v>
@@ -3081,13 +3648,16 @@
       <c r="F84">
         <v>0.03244746077034172</v>
       </c>
-    </row>
-    <row r="85" spans="1:6">
+      <c r="G84">
+        <v>0.03244746077034172</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
       <c r="D85" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E85">
         <v>0.03577073761265144</v>
@@ -3095,13 +3665,16 @@
       <c r="F85">
         <v>0.03577073761265144</v>
       </c>
-    </row>
-    <row r="86" spans="1:6">
+      <c r="G85">
+        <v>0.03577073761265144</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
       <c r="D86" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E86">
         <v>0.0329123907313428</v>
@@ -3109,15 +3682,18 @@
       <c r="F86">
         <v>0.0329123907313428</v>
       </c>
-    </row>
-    <row r="87" spans="1:6">
+      <c r="G86">
+        <v>0.0329123907313428</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1">
         <v>4</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E87">
         <v>1</v>
@@ -3125,13 +3701,16 @@
       <c r="F87">
         <v>1</v>
       </c>
-    </row>
-    <row r="88" spans="1:6">
+      <c r="G87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
       <c r="D88" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E88">
         <v>5.831013606964308</v>
@@ -3139,13 +3718,16 @@
       <c r="F88">
         <v>5.831013606964308</v>
       </c>
-    </row>
-    <row r="89" spans="1:6">
+      <c r="G88">
+        <v>5.831013606964308</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
       <c r="D89" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E89">
         <v>0.08626393627278621</v>
@@ -3153,13 +3735,16 @@
       <c r="F89">
         <v>0.08626393627278621</v>
       </c>
-    </row>
-    <row r="90" spans="1:6">
+      <c r="G89">
+        <v>0.08626393627278621</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
       <c r="D90" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E90">
         <v>0.1029896820652472</v>
@@ -3167,13 +3752,16 @@
       <c r="F90">
         <v>0.1029896820652472</v>
       </c>
-    </row>
-    <row r="91" spans="1:6">
+      <c r="G90">
+        <v>0.1029896820652472</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
       <c r="D91" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E91">
         <v>0.08701145816983205</v>
@@ -3181,15 +3769,18 @@
       <c r="F91">
         <v>0.08701145816983205</v>
       </c>
-    </row>
-    <row r="92" spans="1:6">
+      <c r="G91">
+        <v>0.08701145816983205</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1">
         <v>16</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E92">
         <v>1</v>
@@ -3197,13 +3788,16 @@
       <c r="F92">
         <v>1</v>
       </c>
-    </row>
-    <row r="93" spans="1:6">
+      <c r="G92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
       <c r="D93" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E93">
         <v>1.005778952242822</v>
@@ -3211,13 +3805,16 @@
       <c r="F93">
         <v>1.005778952242822</v>
       </c>
-    </row>
-    <row r="94" spans="1:6">
+      <c r="G93">
+        <v>1.005778952242822</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
       <c r="D94" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E94">
         <v>0.02703107255585205</v>
@@ -3225,13 +3822,16 @@
       <c r="F94">
         <v>0.02703107255585205</v>
       </c>
-    </row>
-    <row r="95" spans="1:6">
+      <c r="G94">
+        <v>0.02703107255585205</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
       <c r="D95" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E95">
         <v>0.02102084514708525</v>
@@ -3239,13 +3839,16 @@
       <c r="F95">
         <v>0.02102084514708525</v>
       </c>
-    </row>
-    <row r="96" spans="1:6">
+      <c r="G95">
+        <v>0.02102084514708525</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
       <c r="D96" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E96">
         <v>0.0176184225849898</v>
@@ -3253,15 +3856,18 @@
       <c r="F96">
         <v>0.0176184225849898</v>
       </c>
-    </row>
-    <row r="97" spans="1:6">
+      <c r="G96">
+        <v>0.0176184225849898</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1">
         <v>64</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E97">
         <v>1</v>
@@ -3269,13 +3875,16 @@
       <c r="F97">
         <v>1</v>
       </c>
-    </row>
-    <row r="98" spans="1:6">
+      <c r="G97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
       <c r="D98" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E98">
         <v>3.137561653328468</v>
@@ -3283,13 +3892,16 @@
       <c r="F98">
         <v>3.137561653328468</v>
       </c>
-    </row>
-    <row r="99" spans="1:6">
+      <c r="G98">
+        <v>3.137561653328468</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
       <c r="D99" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E99">
         <v>0.1160751431410155</v>
@@ -3297,13 +3909,16 @@
       <c r="F99">
         <v>0.1160751431410155</v>
       </c>
-    </row>
-    <row r="100" spans="1:6">
+      <c r="G99">
+        <v>0.1160751431410155</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
       <c r="D100" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E100">
         <v>0.134593172205697</v>
@@ -3311,8 +3926,11 @@
       <c r="F100">
         <v>0.134593172205697</v>
       </c>
-    </row>
-    <row r="101" spans="1:6">
+      <c r="G100">
+        <v>0.134593172205697</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7">
       <c r="A101" s="1"/>
       <c r="B101" s="1">
         <v>2048</v>
@@ -3321,7 +3939,7 @@
         <v>1</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E101">
         <v>1</v>
@@ -3329,13 +3947,16 @@
       <c r="F101">
         <v>1</v>
       </c>
-    </row>
-    <row r="102" spans="1:6">
+      <c r="G101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
       <c r="D102" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E102">
         <v>1.218657383413043</v>
@@ -3343,13 +3964,16 @@
       <c r="F102">
         <v>1.218657383413043</v>
       </c>
-    </row>
-    <row r="103" spans="1:6">
+      <c r="G102">
+        <v>1.218657383413043</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
       <c r="D103" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E103">
         <v>0.01247143669104862</v>
@@ -3357,13 +3981,16 @@
       <c r="F103">
         <v>0.01247143669104862</v>
       </c>
-    </row>
-    <row r="104" spans="1:6">
+      <c r="G103">
+        <v>0.01247143669104862</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
       <c r="D104" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E104">
         <v>0.01662998315878466</v>
@@ -3371,13 +3998,16 @@
       <c r="F104">
         <v>0.01662998315878466</v>
       </c>
-    </row>
-    <row r="105" spans="1:6">
+      <c r="G104">
+        <v>0.01662998315878466</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
       <c r="D105" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E105">
         <v>0.01242844696477945</v>
@@ -3385,15 +4015,18 @@
       <c r="F105">
         <v>0.01242844696477945</v>
       </c>
-    </row>
-    <row r="106" spans="1:6">
+      <c r="G105">
+        <v>0.01242844696477945</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1">
         <v>4</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E106">
         <v>1</v>
@@ -3401,13 +4034,16 @@
       <c r="F106">
         <v>1</v>
       </c>
-    </row>
-    <row r="107" spans="1:6">
+      <c r="G106">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
       <c r="D107" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E107">
         <v>0.883704643805977</v>
@@ -3415,13 +4051,16 @@
       <c r="F107">
         <v>0.883704643805977</v>
       </c>
-    </row>
-    <row r="108" spans="1:6">
+      <c r="G107">
+        <v>0.883704643805977</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
       <c r="D108" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E108">
         <v>0.0118022352129606</v>
@@ -3429,13 +4068,16 @@
       <c r="F108">
         <v>0.0118022352129606</v>
       </c>
-    </row>
-    <row r="109" spans="1:6">
+      <c r="G108">
+        <v>0.0118022352129606</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
       <c r="D109" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E109">
         <v>0.02259074122178853</v>
@@ -3443,13 +4085,16 @@
       <c r="F109">
         <v>0.02259074122178853</v>
       </c>
-    </row>
-    <row r="110" spans="1:6">
+      <c r="G109">
+        <v>0.02259074122178853</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
       <c r="D110" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E110">
         <v>0.01499382940202495</v>
@@ -3457,15 +4102,18 @@
       <c r="F110">
         <v>0.01499382940202495</v>
       </c>
-    </row>
-    <row r="111" spans="1:6">
+      <c r="G110">
+        <v>0.01499382940202495</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1">
         <v>16</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E111">
         <v>1</v>
@@ -3473,13 +4121,16 @@
       <c r="F111">
         <v>1</v>
       </c>
-    </row>
-    <row r="112" spans="1:6">
+      <c r="G111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
       <c r="D112" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E112">
         <v>0.6811302439017147</v>
@@ -3487,13 +4138,16 @@
       <c r="F112">
         <v>0.6811302439017147</v>
       </c>
-    </row>
-    <row r="113" spans="1:6">
+      <c r="G112">
+        <v>0.6811302439017147</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
       <c r="D113" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E113">
         <v>0.02407553767657273</v>
@@ -3501,13 +4155,16 @@
       <c r="F113">
         <v>0.02407553767657273</v>
       </c>
-    </row>
-    <row r="114" spans="1:6">
+      <c r="G113">
+        <v>0.02407553767657273</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
       <c r="D114" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E114">
         <v>0.01743311653022702</v>
@@ -3515,13 +4172,16 @@
       <c r="F114">
         <v>0.01743311653022702</v>
       </c>
-    </row>
-    <row r="115" spans="1:6">
+      <c r="G114">
+        <v>0.01743311653022702</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
       <c r="D115" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E115">
         <v>0.01889136133974725</v>
@@ -3529,15 +4189,18 @@
       <c r="F115">
         <v>0.01889136133974725</v>
       </c>
-    </row>
-    <row r="116" spans="1:6">
+      <c r="G115">
+        <v>0.01889136133974725</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1">
         <v>64</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E116">
         <v>1</v>
@@ -3545,13 +4208,16 @@
       <c r="F116">
         <v>1</v>
       </c>
-    </row>
-    <row r="117" spans="1:6">
+      <c r="G116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
       <c r="D117" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E117">
         <v>3.426278146727916</v>
@@ -3559,13 +4225,16 @@
       <c r="F117">
         <v>3.426278146727916</v>
       </c>
-    </row>
-    <row r="118" spans="1:6">
+      <c r="G117">
+        <v>3.426278146727916</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
       <c r="D118" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E118">
         <v>0.2886671529679412</v>
@@ -3573,13 +4242,16 @@
       <c r="F118">
         <v>0.2886671529679412</v>
       </c>
-    </row>
-    <row r="119" spans="1:6">
+      <c r="G118">
+        <v>0.2886671529679412</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
       <c r="D119" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E119">
         <v>0.1722016754059855</v>
@@ -3587,18 +4259,24 @@
       <c r="F119">
         <v>0.1722016754059855</v>
       </c>
-    </row>
-    <row r="120" spans="1:6">
+      <c r="G119">
+        <v>0.1722016754059855</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
       <c r="D120" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E120">
         <v>0.1752776376515063</v>
       </c>
       <c r="F120">
+        <v>0.1752776376515063</v>
+      </c>
+      <c r="G120">
         <v>0.1752776376515063</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updating summary spreadsheet script and xlsx/csv files
</commit_message>
<xml_diff>
--- a/summary_spreadsheets/multinode_benchmark_results_summary.xlsx
+++ b/summary_spreadsheets/multinode_benchmark_results_summary.xlsx
@@ -7,19 +7,83 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="EchoLeafFederate" sheetId="1" r:id="rId1"/>
-    <sheet name="EchoMessageLeafFederate" sheetId="2" r:id="rId2"/>
-    <sheet name="RingTransmitFederate" sheetId="3" r:id="rId3"/>
-    <sheet name="TimingLeafFederate" sheetId="4" r:id="rId4"/>
-    <sheet name="PholdFederate" sheetId="5" r:id="rId5"/>
-    <sheet name="MessageExchangeFederate" sheetId="6" r:id="rId6"/>
+    <sheet name="CPU Benchmark Score" sheetId="1" r:id="rId1"/>
+    <sheet name="EchoLeafFederate" sheetId="2" r:id="rId2"/>
+    <sheet name="EchoMessageLeafFederate" sheetId="3" r:id="rId3"/>
+    <sheet name="RingTransmitFederate" sheetId="4" r:id="rId4"/>
+    <sheet name="TimingLeafFederate" sheetId="5" r:id="rId5"/>
+    <sheet name="PholdFederate" sheetId="6" r:id="rId6"/>
+    <sheet name="MessageExchangeFederate" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="37">
+  <si>
+    <t>cpe</t>
+  </si>
+  <si>
+    <t>cpf</t>
+  </si>
+  <si>
+    <t>cpmc</t>
+  </si>
+  <si>
+    <t>cpms</t>
+  </si>
+  <si>
+    <t>spe</t>
+  </si>
+  <si>
+    <t>spf</t>
+  </si>
+  <si>
+    <t>spmc</t>
+  </si>
+  <si>
+    <t>spms</t>
+  </si>
+  <si>
+    <t>helics_version_string</t>
+  </si>
+  <si>
+    <t>cpu_score</t>
+  </si>
+  <si>
+    <t>benchmark</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>2.3.1-multinode-phold-benchmark-g0cc2a039 (2020-01-08)</t>
+  </si>
+  <si>
+    <t>2.4.0-base-benchmark-federate-g1e9ac3ab-dirty (2020-02-24)</t>
+  </si>
+  <si>
+    <t>PholdFederate</t>
+  </si>
+  <si>
+    <t>EchoLeafFederate</t>
+  </si>
+  <si>
+    <t>EchoMessageLeafFederate</t>
+  </si>
+  <si>
+    <t>MessageExchangeFederate</t>
+  </si>
+  <si>
+    <t>RingTransmitFederate</t>
+  </si>
+  <si>
+    <t>2020-01-08</t>
+  </si>
+  <si>
+    <t>2020-03-13</t>
+  </si>
   <si>
     <t>elapsed_time_ratio</t>
   </si>
@@ -27,16 +91,10 @@
     <t>spf_ratio</t>
   </si>
   <si>
-    <t>benchmark</t>
-  </si>
-  <si>
     <t>federate_count</t>
   </si>
   <si>
     <t>core_type</t>
-  </si>
-  <si>
-    <t>EchoLeafFederate</t>
   </si>
   <si>
     <t>tcp</t>
@@ -54,12 +112,6 @@
     <t>zmqss</t>
   </si>
   <si>
-    <t>EchoMessageLeafFederate</t>
-  </si>
-  <si>
-    <t>RingTransmitFederate</t>
-  </si>
-  <si>
     <t>cpe_ratio</t>
   </si>
   <si>
@@ -67,9 +119,6 @@
   </si>
   <si>
     <t>spe_ratio</t>
-  </si>
-  <si>
-    <t>PholdFederate</t>
   </si>
   <si>
     <t>spmc_ratio</t>
@@ -82,9 +131,6 @@
   </si>
   <si>
     <t>message_count</t>
-  </si>
-  <si>
-    <t>MessageExchangeFederate</t>
   </si>
 </sst>
 </file>
@@ -442,306 +488,154 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="J1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1">
-        <v>1</v>
+        <v>3185</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
+        <v>14</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="E2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
+        <v>3785.03769302487</v>
+      </c>
+      <c r="F2">
+        <v>12100206.52977462</v>
+      </c>
+      <c r="I2">
+        <v>0.004846278979045912</v>
+      </c>
+      <c r="J2">
+        <v>15.86315858197167</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1">
+        <v>638449</v>
+      </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3">
-        <v>414.2393639987217</v>
-      </c>
-      <c r="E3">
-        <v>414.2393639987217</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>15</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3">
+        <v>22116818.03071701</v>
+      </c>
+      <c r="J3">
+        <v>32.98305247823749</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4">
-        <v>1.028231177573642</v>
-      </c>
-      <c r="E4">
-        <v>1.028231177573642</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4">
+        <v>15393332.7265529</v>
+      </c>
+      <c r="J4">
+        <v>26.31364298958125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5">
-        <v>3.512383880644123</v>
-      </c>
-      <c r="E5">
-        <v>3.512383880644123</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>17</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5">
+        <v>9.939433527109529</v>
+      </c>
+      <c r="H5">
+        <v>8.225906127224377</v>
+      </c>
+      <c r="K5">
+        <v>0.02075071817620797</v>
+      </c>
+      <c r="L5">
+        <v>0.01391972561164406</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6">
-        <v>1.431276638478164</v>
-      </c>
-      <c r="E6">
-        <v>1.431276638478164</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1">
-        <v>2</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8">
-        <v>2.204123275762006</v>
-      </c>
-      <c r="E8">
-        <v>2.204123275762006</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9">
-        <v>0.01118168061816597</v>
-      </c>
-      <c r="E9">
-        <v>0.01118168061816597</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10">
-        <v>0.009739092708668433</v>
-      </c>
-      <c r="E10">
-        <v>0.009739092708668433</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11">
-        <v>0.009385503273635349</v>
-      </c>
-      <c r="E11">
-        <v>0.009385503273635349</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1">
-        <v>4</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13">
-        <v>120.6311428616924</v>
-      </c>
-      <c r="E13">
-        <v>120.6311428616924</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14">
-        <v>1.005046860188864</v>
-      </c>
-      <c r="E14">
-        <v>1.005046860188864</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15">
-        <v>0.6479166653796352</v>
-      </c>
-      <c r="E15">
-        <v>0.6479166653796352</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16">
-        <v>0.6456940956112384</v>
-      </c>
-      <c r="E16">
-        <v>0.6456940956112384</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1">
-        <v>8</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18">
-        <v>23.12031455957467</v>
-      </c>
-      <c r="E18">
-        <v>23.12031455957467</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19">
-        <v>0.3336097501135856</v>
-      </c>
-      <c r="E19">
-        <v>0.3336097501135856</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20">
-        <v>0.1867451589563411</v>
-      </c>
-      <c r="E20">
-        <v>0.1867451589563411</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21">
-        <v>0.1819662395244153</v>
-      </c>
-      <c r="E21">
-        <v>0.1819662395244153</v>
+        <v>18</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6">
+        <v>45653807.20812139</v>
+      </c>
+      <c r="J6">
+        <v>25.79014239635</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A2:A21"/>
-    <mergeCell ref="B2:B6"/>
-    <mergeCell ref="B7:B11"/>
-    <mergeCell ref="B12:B16"/>
-    <mergeCell ref="B17:B21"/>
+  <mergeCells count="2">
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="B3:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -757,30 +651,30 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -793,52 +687,52 @@
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="D3">
-        <v>330.7004734175064</v>
+        <v>414.2393639987217</v>
       </c>
       <c r="E3">
-        <v>330.7004734175064</v>
+        <v>414.2393639987217</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="D4">
-        <v>1.181978885850061</v>
+        <v>1.028231177573642</v>
       </c>
       <c r="E4">
-        <v>1.181978885850061</v>
+        <v>1.028231177573642</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="D5">
-        <v>1.208333321902606</v>
+        <v>3.512383880644123</v>
       </c>
       <c r="E5">
-        <v>1.208333321902606</v>
+        <v>3.512383880644123</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D6">
-        <v>1.266961825925632</v>
+        <v>1.431276638478164</v>
       </c>
       <c r="E6">
-        <v>1.266961825925632</v>
+        <v>1.431276638478164</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -847,7 +741,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -860,52 +754,52 @@
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="D8">
-        <v>231.9685252702395</v>
+        <v>2.204123275762006</v>
       </c>
       <c r="E8">
-        <v>231.9685252702395</v>
+        <v>2.204123275762006</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="D9">
-        <v>1.093423995111745</v>
+        <v>0.01118168061816597</v>
       </c>
       <c r="E9">
-        <v>1.093423995111745</v>
+        <v>0.01118168061816597</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="D10">
-        <v>1.043289373814342</v>
+        <v>0.009739092708668433</v>
       </c>
       <c r="E10">
-        <v>1.043289373814342</v>
+        <v>0.009739092708668433</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D11">
-        <v>0.9435295198866849</v>
+        <v>0.009385503273635349</v>
       </c>
       <c r="E11">
-        <v>0.9435295198866849</v>
+        <v>0.009385503273635349</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -914,7 +808,7 @@
         <v>4</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -927,52 +821,52 @@
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="D13">
-        <v>192.9435269470882</v>
+        <v>120.6311428616924</v>
       </c>
       <c r="E13">
-        <v>192.9435269470882</v>
+        <v>120.6311428616924</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="D14">
-        <v>1.610578780168383</v>
+        <v>1.005046860188864</v>
       </c>
       <c r="E14">
-        <v>1.610578780168383</v>
+        <v>1.005046860188864</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="D15">
-        <v>1.007666280221873</v>
+        <v>0.6479166653796352</v>
       </c>
       <c r="E15">
-        <v>1.007666280221873</v>
+        <v>0.6479166653796352</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D16">
-        <v>1.120033271682305</v>
+        <v>0.6456940956112384</v>
       </c>
       <c r="E16">
-        <v>1.120033271682305</v>
+        <v>0.6456940956112384</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -981,7 +875,7 @@
         <v>8</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -994,52 +888,52 @@
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="D18">
-        <v>100.6712253676607</v>
+        <v>23.12031455957467</v>
       </c>
       <c r="E18">
-        <v>100.6712253676607</v>
+        <v>23.12031455957467</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="D19">
-        <v>1.780722679881865</v>
+        <v>0.3336097501135856</v>
       </c>
       <c r="E19">
-        <v>1.780722679881865</v>
+        <v>0.3336097501135856</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="D20">
-        <v>0.9281915809706429</v>
+        <v>0.1867451589563411</v>
       </c>
       <c r="E20">
-        <v>0.9281915809706429</v>
+        <v>0.1867451589563411</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D21">
-        <v>0.886690641558511</v>
+        <v>0.1819662395244153</v>
       </c>
       <c r="E21">
-        <v>0.886690641558511</v>
+        <v>0.1819662395244153</v>
       </c>
     </row>
   </sheetData>
@@ -1064,30 +958,30 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1100,52 +994,52 @@
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="D3">
-        <v>0.9435639823523477</v>
+        <v>330.7004734175064</v>
       </c>
       <c r="E3">
-        <v>0.9435639823523477</v>
+        <v>330.7004734175064</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="D4">
-        <v>1.060121470154189</v>
+        <v>1.181978885850061</v>
       </c>
       <c r="E4">
-        <v>1.060121470154189</v>
+        <v>1.181978885850061</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="D5">
-        <v>1.064675410041091</v>
+        <v>1.208333321902606</v>
       </c>
       <c r="E5">
-        <v>1.064675410041091</v>
+        <v>1.208333321902606</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D6">
-        <v>0.9682819863115475</v>
+        <v>1.266961825925632</v>
       </c>
       <c r="E6">
-        <v>0.9682819863115475</v>
+        <v>1.266961825925632</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1154,7 +1048,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -1167,52 +1061,52 @@
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="D8">
-        <v>225.9668285269331</v>
+        <v>231.9685252702395</v>
       </c>
       <c r="E8">
-        <v>225.9668285269331</v>
+        <v>231.9685252702395</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="D9">
-        <v>0.9090417806642039</v>
+        <v>1.093423995111745</v>
       </c>
       <c r="E9">
-        <v>0.9090417806642039</v>
+        <v>1.093423995111745</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="D10">
-        <v>4.72454827484734</v>
+        <v>1.043289373814342</v>
       </c>
       <c r="E10">
-        <v>4.72454827484734</v>
+        <v>1.043289373814342</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D11">
-        <v>4.678394481572738</v>
+        <v>0.9435295198866849</v>
       </c>
       <c r="E11">
-        <v>4.678394481572738</v>
+        <v>0.9435295198866849</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1221,7 +1115,7 @@
         <v>4</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -1234,52 +1128,52 @@
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="D13">
-        <v>157.879355478262</v>
+        <v>192.9435269470882</v>
       </c>
       <c r="E13">
-        <v>157.879355478262</v>
+        <v>192.9435269470882</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="D14">
-        <v>0.6731253732532476</v>
+        <v>1.610578780168383</v>
       </c>
       <c r="E14">
-        <v>0.6731253732532476</v>
+        <v>1.610578780168383</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="D15">
-        <v>3.665070623150748</v>
+        <v>1.007666280221873</v>
       </c>
       <c r="E15">
-        <v>3.665070623150748</v>
+        <v>1.007666280221873</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D16">
-        <v>2.938145464950471</v>
+        <v>1.120033271682305</v>
       </c>
       <c r="E16">
-        <v>2.938145464950471</v>
+        <v>1.120033271682305</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1288,7 +1182,7 @@
         <v>8</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -1301,52 +1195,52 @@
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="D18">
-        <v>105.2195177464722</v>
+        <v>100.6712253676607</v>
       </c>
       <c r="E18">
-        <v>105.2195177464722</v>
+        <v>100.6712253676607</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="D19">
-        <v>0.7007826888548608</v>
+        <v>1.780722679881865</v>
       </c>
       <c r="E19">
-        <v>0.7007826888548608</v>
+        <v>1.780722679881865</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="D20">
-        <v>1.806874346148886</v>
+        <v>0.9281915809706429</v>
       </c>
       <c r="E20">
-        <v>1.806874346148886</v>
+        <v>0.9281915809706429</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D21">
-        <v>1.876405585252029</v>
+        <v>0.886690641558511</v>
       </c>
       <c r="E21">
-        <v>1.876405585252029</v>
+        <v>0.886690641558511</v>
       </c>
     </row>
   </sheetData>
@@ -1371,30 +1265,30 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1407,7 +1301,7 @@
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="D3">
         <v>0.9435639823523477</v>
@@ -1420,7 +1314,7 @@
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="D4">
         <v>1.060121470154189</v>
@@ -1433,7 +1327,7 @@
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="D5">
         <v>1.064675410041091</v>
@@ -1446,7 +1340,7 @@
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D6">
         <v>0.9682819863115475</v>
@@ -1461,7 +1355,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -1474,7 +1368,7 @@
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="D8">
         <v>225.9668285269331</v>
@@ -1487,7 +1381,7 @@
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="D9">
         <v>0.9090417806642039</v>
@@ -1500,7 +1394,7 @@
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="D10">
         <v>4.72454827484734</v>
@@ -1513,7 +1407,7 @@
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D11">
         <v>4.678394481572738</v>
@@ -1528,7 +1422,7 @@
         <v>4</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -1541,7 +1435,7 @@
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="D13">
         <v>157.879355478262</v>
@@ -1554,7 +1448,7 @@
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="D14">
         <v>0.6731253732532476</v>
@@ -1567,7 +1461,7 @@
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="D15">
         <v>3.665070623150748</v>
@@ -1580,7 +1474,7 @@
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D16">
         <v>2.938145464950471</v>
@@ -1595,7 +1489,7 @@
         <v>8</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -1608,7 +1502,7 @@
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="D18">
         <v>105.2195177464722</v>
@@ -1621,7 +1515,7 @@
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="D19">
         <v>0.7007826888548608</v>
@@ -1634,7 +1528,7 @@
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="D20">
         <v>1.806874346148886</v>
@@ -1647,7 +1541,7 @@
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D21">
         <v>1.876405585252029</v>
@@ -1670,47 +1564,38 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1718,111 +1603,66 @@
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="D3">
-        <v>1.631098005983478</v>
+        <v>0.9435639823523477</v>
       </c>
       <c r="E3">
-        <v>1.631098005983478</v>
-      </c>
-      <c r="F3">
-        <v>1.277144473418524</v>
-      </c>
-      <c r="G3">
-        <v>1.277144473418524</v>
-      </c>
-      <c r="H3">
-        <v>1.277144473418524</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>0.9435639823523477</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="D4">
-        <v>1.606472437362901</v>
+        <v>1.060121470154189</v>
       </c>
       <c r="E4">
-        <v>1.606472437362902</v>
-      </c>
-      <c r="F4">
-        <v>1.267466937384523</v>
-      </c>
-      <c r="G4">
-        <v>1.267466937384523</v>
-      </c>
-      <c r="H4">
-        <v>1.267466937384523</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>1.060121470154189</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="D5">
-        <v>1.585843969335239</v>
+        <v>1.064675410041091</v>
       </c>
       <c r="E5">
-        <v>1.585843969335239</v>
-      </c>
-      <c r="F5">
-        <v>1.259302969636473</v>
-      </c>
-      <c r="G5">
-        <v>1.259302969636473</v>
-      </c>
-      <c r="H5">
-        <v>1.259302969636473</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>1.064675410041091</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D6">
-        <v>1.872859726645483</v>
+        <v>0.9682819863115475</v>
       </c>
       <c r="E6">
-        <v>1.872859726645483</v>
-      </c>
-      <c r="F6">
-        <v>1.368524653283777</v>
-      </c>
-      <c r="G6">
-        <v>1.368524653283777</v>
-      </c>
-      <c r="H6">
-        <v>1.368524653283777</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>0.9682819863115475</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="1"/>
       <c r="B7" s="1">
         <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -1830,111 +1670,66 @@
       <c r="E7">
         <v>1</v>
       </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="D8">
-        <v>40219.51109919947</v>
+        <v>225.9668285269331</v>
       </c>
       <c r="E8">
-        <v>40219.51109919947</v>
-      </c>
-      <c r="F8">
-        <v>200.5480269006499</v>
-      </c>
-      <c r="G8">
-        <v>200.54802690065</v>
-      </c>
-      <c r="H8">
-        <v>200.54802690065</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>225.9668285269331</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="D9">
-        <v>0.8931655725849961</v>
+        <v>0.9090417806642039</v>
       </c>
       <c r="E9">
-        <v>0.893165572584996</v>
-      </c>
-      <c r="F9">
-        <v>0.9450743738791469</v>
-      </c>
-      <c r="G9">
-        <v>0.9450743738791469</v>
-      </c>
-      <c r="H9">
-        <v>0.9450743738791469</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+        <v>0.9090417806642039</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="D10">
-        <v>1.632792625499382</v>
+        <v>4.72454827484734</v>
       </c>
       <c r="E10">
-        <v>1.632792625499382</v>
-      </c>
-      <c r="F10">
-        <v>1.277807740372132</v>
-      </c>
-      <c r="G10">
-        <v>1.277807740372132</v>
-      </c>
-      <c r="H10">
-        <v>1.277807740372132</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+        <v>4.72454827484734</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D11">
-        <v>1.598918413577855</v>
+        <v>4.678394481572738</v>
       </c>
       <c r="E11">
-        <v>1.598918413577855</v>
-      </c>
-      <c r="F11">
-        <v>1.264483456074377</v>
-      </c>
-      <c r="G11">
-        <v>1.264483456074378</v>
-      </c>
-      <c r="H11">
-        <v>1.264483456074377</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+        <v>4.678394481572738</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="1"/>
       <c r="B12" s="1">
         <v>4</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -1942,111 +1737,66 @@
       <c r="E12">
         <v>1</v>
       </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="D13">
-        <v>16683.52383416874</v>
+        <v>157.879355478262</v>
       </c>
       <c r="E13">
-        <v>16683.52383416874</v>
-      </c>
-      <c r="F13">
-        <v>129.1647156639779</v>
-      </c>
-      <c r="G13">
-        <v>129.1647156639779</v>
-      </c>
-      <c r="H13">
-        <v>129.1647156639779</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+        <v>157.879355478262</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="D14">
-        <v>1.514401343519805</v>
+        <v>0.6731253732532476</v>
       </c>
       <c r="E14">
-        <v>1.514401343519806</v>
-      </c>
-      <c r="F14">
-        <v>1.230610149112736</v>
-      </c>
-      <c r="G14">
-        <v>1.230610149112735</v>
-      </c>
-      <c r="H14">
-        <v>1.230610149112736</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
+        <v>0.6731253732532476</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="D15">
-        <v>2.071497716208372</v>
+        <v>3.665070623150748</v>
       </c>
       <c r="E15">
-        <v>2.071497716208372</v>
-      </c>
-      <c r="F15">
-        <v>1.439269853087512</v>
-      </c>
-      <c r="G15">
-        <v>1.439269853087512</v>
-      </c>
-      <c r="H15">
-        <v>1.439269853087512</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
+        <v>3.665070623150748</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D16">
-        <v>2.88904402681033</v>
+        <v>2.938145464950471</v>
       </c>
       <c r="E16">
-        <v>2.88904402681033</v>
-      </c>
-      <c r="F16">
-        <v>1.699718805686186</v>
-      </c>
-      <c r="G16">
-        <v>1.699718805686186</v>
-      </c>
-      <c r="H16">
-        <v>1.699718805686186</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
+        <v>2.938145464950471</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="1"/>
       <c r="B17" s="1">
         <v>8</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -2054,102 +1804,57 @@
       <c r="E17">
         <v>1</v>
       </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
-      <c r="H17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="D18">
-        <v>6040.81103932062</v>
+        <v>105.2195177464722</v>
       </c>
       <c r="E18">
-        <v>6040.81103932062</v>
-      </c>
-      <c r="F18">
-        <v>77.72265457582611</v>
-      </c>
-      <c r="G18">
-        <v>77.72265457582611</v>
-      </c>
-      <c r="H18">
-        <v>77.72265457582611</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
+        <v>105.2195177464722</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="D19">
-        <v>2.226879116634304</v>
+        <v>0.7007826888548608</v>
       </c>
       <c r="E19">
-        <v>2.226879116634304</v>
-      </c>
-      <c r="F19">
-        <v>1.492273136425073</v>
-      </c>
-      <c r="G19">
-        <v>1.492273136425073</v>
-      </c>
-      <c r="H19">
-        <v>1.492273136425073</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
+        <v>0.7007826888548608</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="D20">
-        <v>2.207722524362522</v>
+        <v>1.806874346148886</v>
       </c>
       <c r="E20">
-        <v>2.207722524362522</v>
-      </c>
-      <c r="F20">
-        <v>1.485840678563465</v>
-      </c>
-      <c r="G20">
-        <v>1.485840678563465</v>
-      </c>
-      <c r="H20">
-        <v>1.485840678563465</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
+        <v>1.806874346148886</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D21">
-        <v>2.516055352821687</v>
+        <v>1.876405585252029</v>
       </c>
       <c r="E21">
-        <v>2.516055352821687</v>
-      </c>
-      <c r="F21">
-        <v>1.586207851736727</v>
-      </c>
-      <c r="G21">
-        <v>1.586207851736727</v>
-      </c>
-      <c r="H21">
-        <v>1.586207851736727</v>
+        <v>1.876405585252029</v>
       </c>
     </row>
   </sheetData>
@@ -2166,6 +1871,502 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3">
+        <v>1.631098005983478</v>
+      </c>
+      <c r="E3">
+        <v>1.631098005983478</v>
+      </c>
+      <c r="F3">
+        <v>1.277144473418524</v>
+      </c>
+      <c r="G3">
+        <v>1.277144473418524</v>
+      </c>
+      <c r="H3">
+        <v>1.277144473418524</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4">
+        <v>1.606472437362901</v>
+      </c>
+      <c r="E4">
+        <v>1.606472437362902</v>
+      </c>
+      <c r="F4">
+        <v>1.267466937384523</v>
+      </c>
+      <c r="G4">
+        <v>1.267466937384523</v>
+      </c>
+      <c r="H4">
+        <v>1.267466937384523</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5">
+        <v>1.585843969335239</v>
+      </c>
+      <c r="E5">
+        <v>1.585843969335239</v>
+      </c>
+      <c r="F5">
+        <v>1.259302969636473</v>
+      </c>
+      <c r="G5">
+        <v>1.259302969636473</v>
+      </c>
+      <c r="H5">
+        <v>1.259302969636473</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6">
+        <v>1.872859726645483</v>
+      </c>
+      <c r="E6">
+        <v>1.872859726645483</v>
+      </c>
+      <c r="F6">
+        <v>1.368524653283777</v>
+      </c>
+      <c r="G6">
+        <v>1.368524653283777</v>
+      </c>
+      <c r="H6">
+        <v>1.368524653283777</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8">
+        <v>40219.51109919947</v>
+      </c>
+      <c r="E8">
+        <v>40219.51109919947</v>
+      </c>
+      <c r="F8">
+        <v>200.5480269006499</v>
+      </c>
+      <c r="G8">
+        <v>200.54802690065</v>
+      </c>
+      <c r="H8">
+        <v>200.54802690065</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9">
+        <v>0.8931655725849961</v>
+      </c>
+      <c r="E9">
+        <v>0.893165572584996</v>
+      </c>
+      <c r="F9">
+        <v>0.9450743738791469</v>
+      </c>
+      <c r="G9">
+        <v>0.9450743738791469</v>
+      </c>
+      <c r="H9">
+        <v>0.9450743738791469</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10">
+        <v>1.632792625499382</v>
+      </c>
+      <c r="E10">
+        <v>1.632792625499382</v>
+      </c>
+      <c r="F10">
+        <v>1.277807740372132</v>
+      </c>
+      <c r="G10">
+        <v>1.277807740372132</v>
+      </c>
+      <c r="H10">
+        <v>1.277807740372132</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11">
+        <v>1.598918413577855</v>
+      </c>
+      <c r="E11">
+        <v>1.598918413577855</v>
+      </c>
+      <c r="F11">
+        <v>1.264483456074377</v>
+      </c>
+      <c r="G11">
+        <v>1.264483456074378</v>
+      </c>
+      <c r="H11">
+        <v>1.264483456074377</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1">
+        <v>4</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13">
+        <v>16683.52383416874</v>
+      </c>
+      <c r="E13">
+        <v>16683.52383416874</v>
+      </c>
+      <c r="F13">
+        <v>129.1647156639779</v>
+      </c>
+      <c r="G13">
+        <v>129.1647156639779</v>
+      </c>
+      <c r="H13">
+        <v>129.1647156639779</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14">
+        <v>1.514401343519805</v>
+      </c>
+      <c r="E14">
+        <v>1.514401343519806</v>
+      </c>
+      <c r="F14">
+        <v>1.230610149112736</v>
+      </c>
+      <c r="G14">
+        <v>1.230610149112735</v>
+      </c>
+      <c r="H14">
+        <v>1.230610149112736</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15">
+        <v>2.071497716208372</v>
+      </c>
+      <c r="E15">
+        <v>2.071497716208372</v>
+      </c>
+      <c r="F15">
+        <v>1.439269853087512</v>
+      </c>
+      <c r="G15">
+        <v>1.439269853087512</v>
+      </c>
+      <c r="H15">
+        <v>1.439269853087512</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16">
+        <v>2.88904402681033</v>
+      </c>
+      <c r="E16">
+        <v>2.88904402681033</v>
+      </c>
+      <c r="F16">
+        <v>1.699718805686186</v>
+      </c>
+      <c r="G16">
+        <v>1.699718805686186</v>
+      </c>
+      <c r="H16">
+        <v>1.699718805686186</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1">
+        <v>8</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18">
+        <v>6040.81103932062</v>
+      </c>
+      <c r="E18">
+        <v>6040.81103932062</v>
+      </c>
+      <c r="F18">
+        <v>77.72265457582611</v>
+      </c>
+      <c r="G18">
+        <v>77.72265457582611</v>
+      </c>
+      <c r="H18">
+        <v>77.72265457582611</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19">
+        <v>2.226879116634304</v>
+      </c>
+      <c r="E19">
+        <v>2.226879116634304</v>
+      </c>
+      <c r="F19">
+        <v>1.492273136425073</v>
+      </c>
+      <c r="G19">
+        <v>1.492273136425073</v>
+      </c>
+      <c r="H19">
+        <v>1.492273136425073</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20">
+        <v>2.207722524362522</v>
+      </c>
+      <c r="E20">
+        <v>2.207722524362522</v>
+      </c>
+      <c r="F20">
+        <v>1.485840678563465</v>
+      </c>
+      <c r="G20">
+        <v>1.485840678563465</v>
+      </c>
+      <c r="H20">
+        <v>1.485840678563465</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21">
+        <v>2.516055352821687</v>
+      </c>
+      <c r="E21">
+        <v>2.516055352821687</v>
+      </c>
+      <c r="F21">
+        <v>1.586207851736727</v>
+      </c>
+      <c r="G21">
+        <v>1.586207851736727</v>
+      </c>
+      <c r="H21">
+        <v>1.586207851736727</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A2:A21"/>
+    <mergeCell ref="B2:B6"/>
+    <mergeCell ref="B7:B11"/>
+    <mergeCell ref="B12:B16"/>
+    <mergeCell ref="B17:B21"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G120"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2174,30 +2375,30 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -2206,7 +2407,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -2223,7 +2424,7 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="E3">
         <v>89.78283223674258</v>
@@ -2240,7 +2441,7 @@
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="E4">
         <v>0.8956669600910819</v>
@@ -2257,7 +2458,7 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="E5">
         <v>1.622970409389778</v>
@@ -2274,7 +2475,7 @@
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="E6">
         <v>1.077075559615454</v>
@@ -2293,7 +2494,7 @@
         <v>4</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -2310,7 +2511,7 @@
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="E8">
         <v>72.83303589992376</v>
@@ -2327,7 +2528,7 @@
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="E9">
         <v>0.8061104475056362</v>
@@ -2344,7 +2545,7 @@
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="E10">
         <v>1.758517619744551</v>
@@ -2361,7 +2562,7 @@
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="E11">
         <v>1.168943875283844</v>
@@ -2380,7 +2581,7 @@
         <v>16</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -2397,7 +2598,7 @@
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="E13">
         <v>67.78463935489476</v>
@@ -2414,7 +2615,7 @@
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="E14">
         <v>2.105372452874108</v>
@@ -2431,7 +2632,7 @@
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="E15">
         <v>1.403689640909411</v>
@@ -2448,7 +2649,7 @@
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="E16">
         <v>1.210800912055891</v>
@@ -2467,7 +2668,7 @@
         <v>64</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -2484,7 +2685,7 @@
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="E18">
         <v>1.68241024430724</v>
@@ -2501,7 +2702,7 @@
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="E19">
         <v>0.1175856896847261</v>
@@ -2518,7 +2719,7 @@
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="E20">
         <v>0.04761894651535323</v>
@@ -2535,7 +2736,7 @@
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="E21">
         <v>0.06243857028336713</v>
@@ -2556,7 +2757,7 @@
         <v>1</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E22">
         <v>1</v>
@@ -2573,7 +2774,7 @@
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="E23">
         <v>114.3223466482583</v>
@@ -2590,7 +2791,7 @@
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="E24">
         <v>1.086597113351394</v>
@@ -2607,7 +2808,7 @@
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="E25">
         <v>1.629422956345736</v>
@@ -2624,7 +2825,7 @@
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="E26">
         <v>1.643552780968021</v>
@@ -2643,7 +2844,7 @@
         <v>4</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E27">
         <v>1</v>
@@ -2660,7 +2861,7 @@
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="E28">
         <v>86.55085846678699</v>
@@ -2677,7 +2878,7 @@
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="E29">
         <v>1.174927066192191</v>
@@ -2694,7 +2895,7 @@
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="E30">
         <v>1.18583941631698</v>
@@ -2711,7 +2912,7 @@
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="E31">
         <v>1.343238987305001</v>
@@ -2730,7 +2931,7 @@
         <v>16</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E32">
         <v>1</v>
@@ -2747,7 +2948,7 @@
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="E33">
         <v>44.87243578827441</v>
@@ -2764,7 +2965,7 @@
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="E34">
         <v>1.825954736924908</v>
@@ -2781,7 +2982,7 @@
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="E35">
         <v>1.07059832111179</v>
@@ -2798,7 +2999,7 @@
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="E36">
         <v>1.058936781932113</v>
@@ -2817,7 +3018,7 @@
         <v>64</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E37">
         <v>1</v>
@@ -2834,7 +3035,7 @@
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="E38">
         <v>8.138883559388573</v>
@@ -2851,7 +3052,7 @@
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="E39">
         <v>0.5189524484568723</v>
@@ -2868,7 +3069,7 @@
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="E40">
         <v>0.2862537280118536</v>
@@ -2885,7 +3086,7 @@
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="E41">
         <v>0.2181377076922102</v>
@@ -2906,7 +3107,7 @@
         <v>1</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E42">
         <v>1</v>
@@ -2923,7 +3124,7 @@
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="E43">
         <v>85.94391614769603</v>
@@ -2940,7 +3141,7 @@
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="E44">
         <v>0.9024757401942765</v>
@@ -2957,7 +3158,7 @@
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="E45">
         <v>2.173957727847946</v>
@@ -2974,7 +3175,7 @@
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="E46">
         <v>1.106434292357325</v>
@@ -2993,7 +3194,7 @@
         <v>4</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E47">
         <v>1</v>
@@ -3010,7 +3211,7 @@
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="E48">
         <v>89.60482592352977</v>
@@ -3027,7 +3228,7 @@
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="E49">
         <v>1.134727682010267</v>
@@ -3044,7 +3245,7 @@
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="E50">
         <v>2.242870346956074</v>
@@ -3061,7 +3262,7 @@
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="E51">
         <v>1.308329054902935</v>
@@ -3080,7 +3281,7 @@
         <v>16</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E52">
         <v>1</v>
@@ -3097,7 +3298,7 @@
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="E53">
         <v>5.572712231505021</v>
@@ -3114,7 +3315,7 @@
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="E54">
         <v>0.1813001785820309</v>
@@ -3131,7 +3332,7 @@
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="E55">
         <v>0.1232298263498409</v>
@@ -3148,7 +3349,7 @@
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="E56">
         <v>0.1078411098594783</v>
@@ -3167,7 +3368,7 @@
         <v>64</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E57">
         <v>1</v>
@@ -3184,7 +3385,7 @@
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="E58">
         <v>1.541367934253603</v>
@@ -3201,7 +3402,7 @@
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="E59">
         <v>0.07219760225253845</v>
@@ -3218,7 +3419,7 @@
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="E60">
         <v>0.03175142187081256</v>
@@ -3235,7 +3436,7 @@
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="E61">
         <v>0.03635015449343772</v>
@@ -3256,7 +3457,7 @@
         <v>1</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E62">
         <v>1</v>
@@ -3273,7 +3474,7 @@
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="E63">
         <v>87.58442267979227</v>
@@ -3290,7 +3491,7 @@
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="E64">
         <v>0.8268447523765605</v>
@@ -3307,7 +3508,7 @@
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="E65">
         <v>1.704276806658666</v>
@@ -3324,7 +3525,7 @@
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="E66">
         <v>1.596775567897026</v>
@@ -3343,7 +3544,7 @@
         <v>4</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E67">
         <v>1</v>
@@ -3360,7 +3561,7 @@
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="E68">
         <v>69.57884361774389</v>
@@ -3377,7 +3578,7 @@
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="E69">
         <v>1.339947959663514</v>
@@ -3394,7 +3595,7 @@
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="E70">
         <v>2.760403364857098</v>
@@ -3411,7 +3612,7 @@
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
       <c r="D71" s="1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="E71">
         <v>1.623740007314907</v>
@@ -3430,7 +3631,7 @@
         <v>16</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E72">
         <v>1</v>
@@ -3447,7 +3648,7 @@
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="E73">
         <v>0.8590609387652602</v>
@@ -3464,7 +3665,7 @@
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="E74">
         <v>0.03445966757525627</v>
@@ -3481,7 +3682,7 @@
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="E75">
         <v>0.02408804393152452</v>
@@ -3498,7 +3699,7 @@
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="E76">
         <v>0.02427279304817658</v>
@@ -3517,7 +3718,7 @@
         <v>64</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E77">
         <v>1</v>
@@ -3534,7 +3735,7 @@
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
       <c r="D78" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="E78">
         <v>1.185151496758129</v>
@@ -3551,7 +3752,7 @@
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
       <c r="D79" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="E79">
         <v>0.05958268897826299</v>
@@ -3568,7 +3769,7 @@
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="E80">
         <v>0.02939762386920262</v>
@@ -3585,7 +3786,7 @@
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
       <c r="D81" s="1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="E81">
         <v>0.03027232211131487</v>
@@ -3606,7 +3807,7 @@
         <v>1</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E82">
         <v>1</v>
@@ -3623,7 +3824,7 @@
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
       <c r="D83" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="E83">
         <v>2.468957735378221</v>
@@ -3640,7 +3841,7 @@
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
       <c r="D84" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="E84">
         <v>0.03244746077034172</v>
@@ -3657,7 +3858,7 @@
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
       <c r="D85" s="1" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="E85">
         <v>0.03577073761265144</v>
@@ -3674,7 +3875,7 @@
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
       <c r="D86" s="1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="E86">
         <v>0.0329123907313428</v>
@@ -3693,7 +3894,7 @@
         <v>4</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E87">
         <v>1</v>
@@ -3710,7 +3911,7 @@
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
       <c r="D88" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="E88">
         <v>5.831013606964308</v>
@@ -3727,7 +3928,7 @@
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
       <c r="D89" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="E89">
         <v>0.08626393627278621</v>
@@ -3744,7 +3945,7 @@
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
       <c r="D90" s="1" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="E90">
         <v>0.1029896820652472</v>
@@ -3761,7 +3962,7 @@
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
       <c r="D91" s="1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="E91">
         <v>0.08701145816983205</v>
@@ -3780,7 +3981,7 @@
         <v>16</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E92">
         <v>1</v>
@@ -3797,7 +3998,7 @@
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
       <c r="D93" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="E93">
         <v>1.005778952242822</v>
@@ -3814,7 +4015,7 @@
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
       <c r="D94" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="E94">
         <v>0.02703107255585205</v>
@@ -3831,7 +4032,7 @@
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
       <c r="D95" s="1" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="E95">
         <v>0.02102084514708525</v>
@@ -3848,7 +4049,7 @@
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
       <c r="D96" s="1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="E96">
         <v>0.0176184225849898</v>
@@ -3867,7 +4068,7 @@
         <v>64</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E97">
         <v>1</v>
@@ -3884,7 +4085,7 @@
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
       <c r="D98" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="E98">
         <v>3.137561653328468</v>
@@ -3901,7 +4102,7 @@
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
       <c r="D99" s="1" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="E99">
         <v>0.1160751431410155</v>
@@ -3918,7 +4119,7 @@
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
       <c r="D100" s="1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="E100">
         <v>0.134593172205697</v>
@@ -3939,7 +4140,7 @@
         <v>1</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E101">
         <v>1</v>
@@ -3956,7 +4157,7 @@
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
       <c r="D102" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="E102">
         <v>1.218657383413043</v>
@@ -3973,7 +4174,7 @@
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
       <c r="D103" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="E103">
         <v>0.01247143669104862</v>
@@ -3990,7 +4191,7 @@
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
       <c r="D104" s="1" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="E104">
         <v>0.01662998315878466</v>
@@ -4007,7 +4208,7 @@
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
       <c r="D105" s="1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="E105">
         <v>0.01242844696477945</v>
@@ -4026,7 +4227,7 @@
         <v>4</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E106">
         <v>1</v>
@@ -4043,7 +4244,7 @@
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
       <c r="D107" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="E107">
         <v>0.883704643805977</v>
@@ -4060,7 +4261,7 @@
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
       <c r="D108" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="E108">
         <v>0.0118022352129606</v>
@@ -4077,7 +4278,7 @@
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
       <c r="D109" s="1" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="E109">
         <v>0.02259074122178853</v>
@@ -4094,7 +4295,7 @@
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
       <c r="D110" s="1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="E110">
         <v>0.01499382940202495</v>
@@ -4113,7 +4314,7 @@
         <v>16</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E111">
         <v>1</v>
@@ -4130,7 +4331,7 @@
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
       <c r="D112" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="E112">
         <v>0.6811302439017147</v>
@@ -4147,7 +4348,7 @@
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
       <c r="D113" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="E113">
         <v>0.02407553767657273</v>
@@ -4164,7 +4365,7 @@
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
       <c r="D114" s="1" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="E114">
         <v>0.01743311653022702</v>
@@ -4181,7 +4382,7 @@
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
       <c r="D115" s="1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="E115">
         <v>0.01889136133974725</v>
@@ -4200,7 +4401,7 @@
         <v>64</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E116">
         <v>1</v>
@@ -4217,7 +4418,7 @@
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
       <c r="D117" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="E117">
         <v>3.426278146727916</v>
@@ -4234,7 +4435,7 @@
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
       <c r="D118" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="E118">
         <v>0.2886671529679412</v>
@@ -4251,7 +4452,7 @@
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
       <c r="D119" s="1" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="E119">
         <v>0.1722016754059855</v>
@@ -4268,7 +4469,7 @@
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
       <c r="D120" s="1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="E120">
         <v>0.1752776376515063</v>

</xml_diff>

<commit_message>
updating summary spreadsheets and csvs and adding a metadata table for each.
</commit_message>
<xml_diff>
--- a/summary_spreadsheets/multinode_benchmark_results_summary.xlsx
+++ b/summary_spreadsheets/multinode_benchmark_results_summary.xlsx
@@ -537,7 +537,7 @@
         <v>12</v>
       </c>
       <c r="B2" s="1">
-        <v>3185</v>
+        <v>1592</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>14</v>
@@ -563,7 +563,7 @@
         <v>13</v>
       </c>
       <c r="B3" s="1">
-        <v>638449</v>
+        <v>319225</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
fixing bug of incorrect data type and updating reports and images
</commit_message>
<xml_diff>
--- a/summary_spreadsheets/multinode_benchmark_results_summary.xlsx
+++ b/summary_spreadsheets/multinode_benchmark_results_summary.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="46">
   <si>
     <t>cpe</t>
   </si>
@@ -107,21 +107,6 @@
     <t>EchoLeafFederate</t>
   </si>
   <si>
-    <t>1.0</t>
-  </si>
-  <si>
-    <t>2.0</t>
-  </si>
-  <si>
-    <t>3.0</t>
-  </si>
-  <si>
-    <t>4.0</t>
-  </si>
-  <si>
-    <t>8.0</t>
-  </si>
-  <si>
     <t>tcp</t>
   </si>
   <si>
@@ -159,18 +144,6 @@
   </si>
   <si>
     <t>PholdFederate</t>
-  </si>
-  <si>
-    <t>16.0</t>
-  </si>
-  <si>
-    <t>18.0</t>
-  </si>
-  <si>
-    <t>36.0</t>
-  </si>
-  <si>
-    <t>72.0</t>
   </si>
   <si>
     <t>spmc_ratio</t>
@@ -682,7 +655,7 @@
         <v>19</v>
       </c>
       <c r="D5">
-        <v>70.20564651344394</v>
+        <v>70.20564651344391</v>
       </c>
       <c r="E5">
         <v>19143.27181222365</v>
@@ -691,7 +664,7 @@
         <v>0.001347534679399217</v>
       </c>
       <c r="I5">
-        <v>0.4486283216425285</v>
+        <v>0.4486283216425289</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -755,10 +728,10 @@
         <v>19</v>
       </c>
       <c r="D8">
-        <v>5.258524819314344</v>
+        <v>5.258524819314339</v>
       </c>
       <c r="E8">
-        <v>8414.726767874561</v>
+        <v>8414.726767874559</v>
       </c>
       <c r="H8">
         <v>0.0003288058304356864</v>
@@ -807,11 +780,11 @@
       <c r="A2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>28</v>
+      <c r="B2" s="1">
+        <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D2">
         <v>0.9999039432951805</v>
@@ -824,7 +797,7 @@
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D3">
         <v>220.661597348397</v>
@@ -837,7 +810,7 @@
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D4">
         <v>0.7910942441318073</v>
@@ -850,7 +823,7 @@
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D5">
         <v>2.097325834303735</v>
@@ -863,7 +836,7 @@
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D6">
         <v>1.320573317283176</v>
@@ -874,11 +847,11 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1"/>
-      <c r="B7" s="1" t="s">
-        <v>29</v>
+      <c r="B7" s="1">
+        <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D7">
         <v>0.9999069920993229</v>
@@ -891,7 +864,7 @@
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D8">
         <v>78.74290565340793</v>
@@ -904,7 +877,7 @@
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D9">
         <v>0.5661889772027642</v>
@@ -917,7 +890,7 @@
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D10">
         <v>0.5582238838350786</v>
@@ -930,7 +903,7 @@
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D11">
         <v>0.6645431832348884</v>
@@ -941,11 +914,11 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="1"/>
-      <c r="B12" s="1" t="s">
-        <v>30</v>
+      <c r="B12" s="1">
+        <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D12">
         <v>0.9998576799266208</v>
@@ -958,7 +931,7 @@
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D13">
         <v>30.81574467829372</v>
@@ -971,7 +944,7 @@
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D14">
         <v>0.6811741605937497</v>
@@ -984,7 +957,7 @@
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D15">
         <v>0.6919494596440523</v>
@@ -997,7 +970,7 @@
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D16">
         <v>0.7230215059360829</v>
@@ -1008,11 +981,11 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="1"/>
-      <c r="B17" s="1" t="s">
-        <v>31</v>
+      <c r="B17" s="1">
+        <v>4</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D17">
         <v>0.9998982171036233</v>
@@ -1025,7 +998,7 @@
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D18">
         <v>88.49021067780581</v>
@@ -1038,7 +1011,7 @@
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D19">
         <v>0.8789519597440254</v>
@@ -1051,7 +1024,7 @@
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D20">
         <v>0.6676409847603774</v>
@@ -1064,7 +1037,7 @@
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D21">
         <v>0.676425587423033</v>
@@ -1075,11 +1048,11 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="1"/>
-      <c r="B22" s="1" t="s">
-        <v>32</v>
+      <c r="B22" s="1">
+        <v>8</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D22">
         <v>0.9999853821037576</v>
@@ -1092,7 +1065,7 @@
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D23">
         <v>17.42018703377445</v>
@@ -1105,7 +1078,7 @@
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D24">
         <v>0.2550104600347619</v>
@@ -1118,7 +1091,7 @@
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D25">
         <v>0.1459320685592806</v>
@@ -1131,7 +1104,7 @@
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D26">
         <v>0.1476603986262623</v>
@@ -1180,13 +1153,13 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D2">
         <v>0.9998762041615548</v>
@@ -1199,7 +1172,7 @@
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D3">
         <v>220.3938051974069</v>
@@ -1212,7 +1185,7 @@
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D4">
         <v>1.00057280749867</v>
@@ -1225,7 +1198,7 @@
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D5">
         <v>1.184002416998598</v>
@@ -1238,7 +1211,7 @@
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D6">
         <v>1.139760880471385</v>
@@ -1249,11 +1222,11 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1"/>
-      <c r="B7" s="1" t="s">
-        <v>29</v>
+      <c r="B7" s="1">
+        <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D7">
         <v>0.9998878646343942</v>
@@ -1266,7 +1239,7 @@
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D8">
         <v>148.7897133246362</v>
@@ -1279,7 +1252,7 @@
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D9">
         <v>0.782617942839319</v>
@@ -1292,7 +1265,7 @@
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D10">
         <v>0.7146603717748289</v>
@@ -1305,7 +1278,7 @@
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D11">
         <v>0.6814116308371411</v>
@@ -1316,11 +1289,11 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="1"/>
-      <c r="B12" s="1" t="s">
-        <v>30</v>
+      <c r="B12" s="1">
+        <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D12">
         <v>0.9997874336423298</v>
@@ -1333,7 +1306,7 @@
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D13">
         <v>25.93174540966189</v>
@@ -1346,7 +1319,7 @@
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D14">
         <v>0.6675873283123595</v>
@@ -1359,7 +1332,7 @@
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D15">
         <v>0.6493770908555183</v>
@@ -1370,11 +1343,11 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="1"/>
-      <c r="B16" s="1" t="s">
-        <v>31</v>
+      <c r="B16" s="1">
+        <v>4</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D16">
         <v>0.9997332670755452</v>
@@ -1387,7 +1360,7 @@
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D17">
         <v>124.3707001026792</v>
@@ -1400,7 +1373,7 @@
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D18">
         <v>1.706311243580039</v>
@@ -1413,7 +1386,7 @@
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D19">
         <v>0.99512834472809</v>
@@ -1426,7 +1399,7 @@
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D20">
         <v>0.9905461867302304</v>
@@ -1437,11 +1410,11 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="1"/>
-      <c r="B21" s="1" t="s">
-        <v>32</v>
+      <c r="B21" s="1">
+        <v>8</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D21">
         <v>0.9998556039683437</v>
@@ -1454,7 +1427,7 @@
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D22">
         <v>51.3044078998788</v>
@@ -1467,7 +1440,7 @@
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D23">
         <v>0.9110176571920792</v>
@@ -1480,7 +1453,7 @@
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D24">
         <v>0.4747919344612661</v>
@@ -1493,7 +1466,7 @@
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D25">
         <v>0.4549050327405202</v>
@@ -1542,13 +1515,13 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>28</v>
+        <v>34</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1561,7 +1534,7 @@
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D3">
         <v>0.9839006721131867</v>
@@ -1574,7 +1547,7 @@
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D4">
         <v>1.024578679601809</v>
@@ -1587,7 +1560,7 @@
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D5">
         <v>0.9950584617490345</v>
@@ -1600,7 +1573,7 @@
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D6">
         <v>1.020577920088135</v>
@@ -1611,11 +1584,11 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1"/>
-      <c r="B7" s="1" t="s">
-        <v>29</v>
+      <c r="B7" s="1">
+        <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D7">
         <v>1.000024358663012</v>
@@ -1628,7 +1601,7 @@
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D8">
         <v>150.2322089087025</v>
@@ -1641,7 +1614,7 @@
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D9">
         <v>0.8178528452484696</v>
@@ -1654,7 +1627,7 @@
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D10">
         <v>2.604161616982373</v>
@@ -1667,7 +1640,7 @@
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D11">
         <v>2.977363483529877</v>
@@ -1678,11 +1651,11 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="1"/>
-      <c r="B12" s="1" t="s">
-        <v>30</v>
+      <c r="B12" s="1">
+        <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D12">
         <v>1.000020507838224</v>
@@ -1695,7 +1668,7 @@
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D13">
         <v>52.49239316892709</v>
@@ -1708,7 +1681,7 @@
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D14">
         <v>0.7193569307081266</v>
@@ -1721,7 +1694,7 @@
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D15">
         <v>0.9734665734530431</v>
@@ -1734,7 +1707,7 @@
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D16">
         <v>1.005268586582202</v>
@@ -1745,11 +1718,11 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="1"/>
-      <c r="B17" s="1" t="s">
-        <v>31</v>
+      <c r="B17" s="1">
+        <v>4</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D17">
         <v>0.9999738357799023</v>
@@ -1762,7 +1735,7 @@
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D18">
         <v>158.0210075406374</v>
@@ -1775,7 +1748,7 @@
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D19">
         <v>0.7758888095256741</v>
@@ -1788,7 +1761,7 @@
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D20">
         <v>2.751370321007433</v>
@@ -1801,7 +1774,7 @@
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D21">
         <v>2.424816621202747</v>
@@ -1812,11 +1785,11 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="1"/>
-      <c r="B22" s="1" t="s">
-        <v>32</v>
+      <c r="B22" s="1">
+        <v>8</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D22">
         <v>0.9999404332515149</v>
@@ -1829,7 +1802,7 @@
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D23">
         <v>102.2118340314646</v>
@@ -1842,7 +1815,7 @@
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D24">
         <v>0.7201540816177607</v>
@@ -1855,7 +1828,7 @@
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D25">
         <v>2.094332691560599</v>
@@ -1868,7 +1841,7 @@
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D26">
         <v>1.915947739281052</v>
@@ -1917,13 +1890,13 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1936,7 +1909,7 @@
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D3">
         <v>0.9616554284613794</v>
@@ -1949,7 +1922,7 @@
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D4">
         <v>0.9394550686392151</v>
@@ -1962,7 +1935,7 @@
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D5">
         <v>0.9207606703488924</v>
@@ -1975,7 +1948,7 @@
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D6">
         <v>0.9398278675649501</v>
@@ -1986,11 +1959,11 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1"/>
-      <c r="B7" s="1" t="s">
-        <v>29</v>
+      <c r="B7" s="1">
+        <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D7">
         <v>0.9999520932624699</v>
@@ -2003,7 +1976,7 @@
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D8">
         <v>81.26965835521783</v>
@@ -2016,7 +1989,7 @@
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D9">
         <v>1.043486139909651</v>
@@ -2029,7 +2002,7 @@
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D10">
         <v>1.070455326654049</v>
@@ -2042,7 +2015,7 @@
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D11">
         <v>1.103550352875533</v>
@@ -2053,11 +2026,11 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="1"/>
-      <c r="B12" s="1" t="s">
-        <v>30</v>
+      <c r="B12" s="1">
+        <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D12">
         <v>0.9998427545762807</v>
@@ -2070,7 +2043,7 @@
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D13">
         <v>22.97492036482046</v>
@@ -2083,7 +2056,7 @@
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D14">
         <v>0.8119896047052636</v>
@@ -2096,7 +2069,7 @@
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D15">
         <v>1.075974983488679</v>
@@ -2109,7 +2082,7 @@
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D16">
         <v>1.085429177539295</v>
@@ -2120,11 +2093,11 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="1"/>
-      <c r="B17" s="1" t="s">
-        <v>31</v>
+      <c r="B17" s="1">
+        <v>4</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D17">
         <v>0.9999576658513551</v>
@@ -2137,7 +2110,7 @@
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D18">
         <v>26.16494268247078</v>
@@ -2150,7 +2123,7 @@
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D19">
         <v>0.6027202059002593</v>
@@ -2163,7 +2136,7 @@
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D20">
         <v>0.6778570661313643</v>
@@ -2176,7 +2149,7 @@
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D21">
         <v>0.6705700647772025</v>
@@ -2187,11 +2160,11 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="1"/>
-      <c r="B22" s="1" t="s">
-        <v>32</v>
+      <c r="B22" s="1">
+        <v>8</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D22">
         <v>0.999936454238274</v>
@@ -2204,7 +2177,7 @@
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D23">
         <v>67.27027781474584</v>
@@ -2217,7 +2190,7 @@
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D24">
         <v>1.772628812296618</v>
@@ -2230,7 +2203,7 @@
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D25">
         <v>0.9577058501617526</v>
@@ -2243,7 +2216,7 @@
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D26">
         <v>0.9777052777666783</v>
@@ -2292,13 +2265,13 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>28</v>
+        <v>36</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D2">
         <v>3.615910984777779</v>
@@ -2311,7 +2284,7 @@
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D3">
         <v>207.342911686</v>
@@ -2324,7 +2297,7 @@
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D4">
         <v>4.578355064999999</v>
@@ -2337,7 +2310,7 @@
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D5">
         <v>3.310436535444445</v>
@@ -2350,7 +2323,7 @@
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D6">
         <v>3.341208269722223</v>
@@ -2361,11 +2334,11 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1"/>
-      <c r="B7" s="1" t="s">
-        <v>29</v>
+      <c r="B7" s="1">
+        <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D7">
         <v>0.9999216147434186</v>
@@ -2378,7 +2351,7 @@
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D8">
         <v>61.75484429461458</v>
@@ -2391,7 +2364,7 @@
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D9">
         <v>0.555808013622035</v>
@@ -2404,7 +2377,7 @@
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D10">
         <v>1.535761941057705</v>
@@ -2417,7 +2390,7 @@
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D11">
         <v>1.243874347497926</v>
@@ -2428,11 +2401,11 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="1"/>
-      <c r="B12" s="1" t="s">
-        <v>30</v>
+      <c r="B12" s="1">
+        <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D12">
         <v>0.9998176192387387</v>
@@ -2445,7 +2418,7 @@
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D13">
         <v>26.04449472854477</v>
@@ -2458,7 +2431,7 @@
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D14">
         <v>0.6933198079374806</v>
@@ -2471,7 +2444,7 @@
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D15">
         <v>0.9260235983116545</v>
@@ -2482,11 +2455,11 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="1"/>
-      <c r="B16" s="1" t="s">
-        <v>31</v>
+      <c r="B16" s="1">
+        <v>4</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D16">
         <v>0.9998590076825564</v>
@@ -2499,7 +2472,7 @@
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D17">
         <v>96.78913157882855</v>
@@ -2512,7 +2485,7 @@
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D18">
         <v>1.171432872834904</v>
@@ -2525,7 +2498,7 @@
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D19">
         <v>2.791270001084853</v>
@@ -2538,7 +2511,7 @@
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D20">
         <v>2.30087968014393</v>
@@ -2549,11 +2522,11 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="1"/>
-      <c r="B21" s="1" t="s">
-        <v>32</v>
+      <c r="B21" s="1">
+        <v>8</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D21">
         <v>0.999928798313754</v>
@@ -2566,7 +2539,7 @@
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D22">
         <v>80.08294047725893</v>
@@ -2579,7 +2552,7 @@
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D23">
         <v>1.092916493088006</v>
@@ -2592,7 +2565,7 @@
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D24">
         <v>1.168374458606502</v>
@@ -2605,7 +2578,7 @@
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D25">
         <v>1.334488510890445</v>
@@ -2646,16 +2619,16 @@
         <v>26</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>22</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>23</v>
@@ -2663,600 +2636,600 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D2">
-        <v>1.072603039920157</v>
+        <v>1.047647477739662</v>
       </c>
       <c r="E2">
-        <v>1.072603039920157</v>
+        <v>1.047647477739662</v>
       </c>
       <c r="F2">
-        <v>1.0350715091294</v>
+        <v>1.02328170119341</v>
       </c>
       <c r="G2">
-        <v>1.0350715091294</v>
+        <v>1.02328170119341</v>
       </c>
       <c r="H2">
-        <v>1.0350715091294</v>
+        <v>1.02328170119341</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D3">
-        <v>1.434620263001065</v>
+        <v>1.027069011876976</v>
       </c>
       <c r="E3">
-        <v>1.434620263001064</v>
+        <v>1.027069011876976</v>
       </c>
       <c r="F3">
-        <v>1.194444850878163</v>
+        <v>1.012918976101511</v>
       </c>
       <c r="G3">
-        <v>1.194444850878163</v>
+        <v>1.012918976101511</v>
       </c>
       <c r="H3">
-        <v>1.194444850878163</v>
+        <v>1.012918976101511</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D4">
-        <v>1.132340154471698</v>
+        <v>1.847896951183879</v>
       </c>
       <c r="E4">
-        <v>1.132340154471698</v>
+        <v>1.84789695118388</v>
       </c>
       <c r="F4">
-        <v>1.063943793357675</v>
+        <v>1.35687533668366</v>
       </c>
       <c r="G4">
-        <v>1.063943793357675</v>
+        <v>1.35687533668366</v>
       </c>
       <c r="H4">
-        <v>1.063943793357675</v>
+        <v>1.356875336683661</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D5">
-        <v>1.126385547587938</v>
+        <v>1.801379113319929</v>
       </c>
       <c r="E5">
-        <v>1.126385547587938</v>
+        <v>1.801379113319929</v>
       </c>
       <c r="F5">
-        <v>1.061228059856178</v>
+        <v>1.339266724082049</v>
       </c>
       <c r="G5">
-        <v>1.061228059856177</v>
+        <v>1.339266724082049</v>
       </c>
       <c r="H5">
-        <v>1.061228059856177</v>
+        <v>1.339266724082049</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1"/>
-      <c r="B6" s="1" t="s">
-        <v>47</v>
+      <c r="B6" s="1">
+        <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D6">
-        <v>1.395273032617649</v>
+        <v>1.143950202582259</v>
       </c>
       <c r="E6">
-        <v>1.395273032617649</v>
+        <v>1.143950202582259</v>
       </c>
       <c r="F6">
-        <v>1.174591275998046</v>
+        <v>1.06742849879104</v>
       </c>
       <c r="G6">
-        <v>1.174591275998046</v>
+        <v>1.06742849879104</v>
       </c>
       <c r="H6">
-        <v>1.174591275998046</v>
+        <v>1.06742849879104</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D7">
-        <v>1.461733340833844</v>
+        <v>1.4163032460703</v>
       </c>
       <c r="E7">
-        <v>1.461733340833844</v>
+        <v>1.4163032460703</v>
       </c>
       <c r="F7">
-        <v>1.198091532034471</v>
+        <v>1.188433684940858</v>
       </c>
       <c r="G7">
-        <v>1.198091532034472</v>
+        <v>1.188433684940858</v>
       </c>
       <c r="H7">
-        <v>1.198091532034472</v>
+        <v>1.188433684940858</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
+      <c r="B8" s="1">
+        <v>8</v>
+      </c>
       <c r="C8" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D8">
-        <v>1.178956978715834</v>
+        <v>0.9714704193393734</v>
       </c>
       <c r="E8">
-        <v>1.178956978715834</v>
+        <v>0.9714704193393734</v>
       </c>
       <c r="F8">
-        <v>1.083840234488519</v>
+        <v>0.9854420345685541</v>
       </c>
       <c r="G8">
-        <v>1.083840234488519</v>
+        <v>0.9854420345685537</v>
       </c>
       <c r="H8">
-        <v>1.083840234488519</v>
+        <v>0.9854420345685537</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D9">
-        <v>1.428165144890509</v>
+        <v>1.156507426534088</v>
       </c>
       <c r="E9">
-        <v>1.428165144890509</v>
+        <v>1.156507426534088</v>
       </c>
       <c r="F9">
-        <v>1.191385845815945</v>
+        <v>1.073863846931256</v>
       </c>
       <c r="G9">
-        <v>1.191385845815946</v>
+        <v>1.073863846931255</v>
       </c>
       <c r="H9">
-        <v>1.191385845815946</v>
+        <v>1.073863846931255</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1"/>
-      <c r="B10" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D10">
-        <v>1.047647477739662</v>
+        <v>1.327493129642546</v>
       </c>
       <c r="E10">
-        <v>1.047647477739662</v>
+        <v>1.327493129642547</v>
       </c>
       <c r="F10">
-        <v>1.02328170119341</v>
+        <v>1.151944994154603</v>
       </c>
       <c r="G10">
-        <v>1.02328170119341</v>
+        <v>1.151944994154604</v>
       </c>
       <c r="H10">
-        <v>1.02328170119341</v>
+        <v>1.151944994154604</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D11">
-        <v>1.027069011876976</v>
+        <v>1.312036687250888</v>
       </c>
       <c r="E11">
-        <v>1.027069011876976</v>
+        <v>1.312036687250888</v>
       </c>
       <c r="F11">
-        <v>1.012918976101511</v>
+        <v>1.145413037702157</v>
       </c>
       <c r="G11">
-        <v>1.012918976101511</v>
+        <v>1.145413037702156</v>
       </c>
       <c r="H11">
-        <v>1.012918976101511</v>
+        <v>1.145413037702156</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
+      <c r="B12" s="1">
+        <v>16</v>
+      </c>
       <c r="C12" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D12">
-        <v>1.847896951183879</v>
+        <v>1.072603039920157</v>
       </c>
       <c r="E12">
-        <v>1.84789695118388</v>
+        <v>1.072603039920157</v>
       </c>
       <c r="F12">
-        <v>1.35687533668366</v>
+        <v>1.0350715091294</v>
       </c>
       <c r="G12">
-        <v>1.35687533668366</v>
+        <v>1.0350715091294</v>
       </c>
       <c r="H12">
-        <v>1.356875336683661</v>
+        <v>1.0350715091294</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D13">
-        <v>1.801379113319929</v>
+        <v>1.434620263001065</v>
       </c>
       <c r="E13">
-        <v>1.801379113319929</v>
+        <v>1.434620263001064</v>
       </c>
       <c r="F13">
-        <v>1.339266724082049</v>
+        <v>1.194444850878163</v>
       </c>
       <c r="G13">
-        <v>1.339266724082049</v>
+        <v>1.194444850878163</v>
       </c>
       <c r="H13">
-        <v>1.339266724082049</v>
+        <v>1.194444850878163</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1"/>
-      <c r="B14" s="1" t="s">
-        <v>48</v>
-      </c>
+      <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D14">
-        <v>0.9449878541868321</v>
+        <v>1.132340154471698</v>
       </c>
       <c r="E14">
-        <v>0.9449878541868321</v>
+        <v>1.132340154471698</v>
       </c>
       <c r="F14">
-        <v>0.967384176779</v>
+        <v>1.063943793357675</v>
       </c>
       <c r="G14">
-        <v>0.967384176779</v>
+        <v>1.063943793357675</v>
       </c>
       <c r="H14">
-        <v>0.967384176779</v>
+        <v>1.063943793357675</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D15">
-        <v>0.9675616585698147</v>
+        <v>1.126385547587938</v>
       </c>
       <c r="E15">
-        <v>0.9675616585698149</v>
+        <v>1.126385547587938</v>
       </c>
       <c r="F15">
-        <v>0.9793658883650725</v>
+        <v>1.061228059856178</v>
       </c>
       <c r="G15">
-        <v>0.9793658883650723</v>
+        <v>1.061228059856177</v>
       </c>
       <c r="H15">
-        <v>0.9793658883650723</v>
+        <v>1.061228059856177</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
+      <c r="B16" s="1">
+        <v>18</v>
+      </c>
       <c r="C16" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D16">
-        <v>0.8334331510230607</v>
+        <v>1.395273032617649</v>
       </c>
       <c r="E16">
-        <v>0.8334331510230608</v>
+        <v>1.395273032617649</v>
       </c>
       <c r="F16">
-        <v>0.9118333519658902</v>
+        <v>1.174591275998046</v>
       </c>
       <c r="G16">
-        <v>0.9118333519658894</v>
+        <v>1.174591275998046</v>
       </c>
       <c r="H16">
-        <v>0.9118333519658894</v>
+        <v>1.174591275998046</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D17">
-        <v>0.854794184916075</v>
+        <v>1.461733340833844</v>
       </c>
       <c r="E17">
-        <v>0.8547941849160748</v>
+        <v>1.461733340833844</v>
       </c>
       <c r="F17">
-        <v>0.9220555810920668</v>
+        <v>1.198091532034471</v>
       </c>
       <c r="G17">
-        <v>0.9220555810920664</v>
+        <v>1.198091532034472</v>
       </c>
       <c r="H17">
-        <v>0.9220555810920664</v>
+        <v>1.198091532034472</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="1"/>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="D18">
-        <v>1.143950202582259</v>
+        <v>1.178956978715834</v>
       </c>
       <c r="E18">
-        <v>1.143950202582259</v>
+        <v>1.178956978715834</v>
       </c>
       <c r="F18">
-        <v>1.06742849879104</v>
+        <v>1.083840234488519</v>
       </c>
       <c r="G18">
-        <v>1.06742849879104</v>
+        <v>1.083840234488519</v>
       </c>
       <c r="H18">
-        <v>1.06742849879104</v>
+        <v>1.083840234488519</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D19">
-        <v>1.4163032460703</v>
+        <v>1.428165144890509</v>
       </c>
       <c r="E19">
-        <v>1.4163032460703</v>
+        <v>1.428165144890509</v>
       </c>
       <c r="F19">
-        <v>1.188433684940858</v>
+        <v>1.191385845815945</v>
       </c>
       <c r="G19">
-        <v>1.188433684940858</v>
+        <v>1.191385845815946</v>
       </c>
       <c r="H19">
-        <v>1.188433684940858</v>
+        <v>1.191385845815946</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="1"/>
-      <c r="B20" s="1" t="s">
-        <v>49</v>
+      <c r="B20" s="1">
+        <v>36</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D20">
-        <v>0.9898927854180372</v>
+        <v>0.9449878541868321</v>
       </c>
       <c r="E20">
-        <v>0.9898927854180372</v>
+        <v>0.9449878541868321</v>
       </c>
       <c r="F20">
-        <v>0.9922843711096743</v>
+        <v>0.967384176779</v>
       </c>
       <c r="G20">
-        <v>0.9922843711096754</v>
+        <v>0.967384176779</v>
       </c>
       <c r="H20">
-        <v>0.9922843711096754</v>
+        <v>0.967384176779</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D21">
-        <v>0.9312482317462356</v>
+        <v>0.9675616585698147</v>
       </c>
       <c r="E21">
-        <v>0.9312482317462357</v>
+        <v>0.9675616585698149</v>
       </c>
       <c r="F21">
-        <v>0.9602283340866721</v>
+        <v>0.9793658883650725</v>
       </c>
       <c r="G21">
-        <v>0.9602283340866712</v>
+        <v>0.9793658883650723</v>
       </c>
       <c r="H21">
-        <v>0.9602283340866712</v>
+        <v>0.9793658883650723</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D22">
-        <v>0.8518766552821998</v>
+        <v>0.8334331510230607</v>
       </c>
       <c r="E22">
-        <v>0.8518766552821998</v>
+        <v>0.8334331510230608</v>
       </c>
       <c r="F22">
-        <v>0.9203297228677866</v>
+        <v>0.9118333519658902</v>
       </c>
       <c r="G22">
-        <v>0.920329722867786</v>
+        <v>0.9118333519658894</v>
       </c>
       <c r="H22">
-        <v>0.920329722867786</v>
+        <v>0.9118333519658894</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D23">
-        <v>0.8258684171300312</v>
+        <v>0.854794184916075</v>
       </c>
       <c r="E23">
-        <v>0.8258684171300312</v>
+        <v>0.8547941849160748</v>
       </c>
       <c r="F23">
-        <v>0.9060760259412903</v>
+        <v>0.9220555810920668</v>
       </c>
       <c r="G23">
-        <v>0.9060760259412913</v>
+        <v>0.9220555810920664</v>
       </c>
       <c r="H23">
-        <v>0.9060760259412913</v>
+        <v>0.9220555810920664</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="1"/>
-      <c r="B24" s="1" t="s">
-        <v>32</v>
+      <c r="B24" s="1">
+        <v>72</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D24">
-        <v>0.9714704193393734</v>
+        <v>0.9898927854180372</v>
       </c>
       <c r="E24">
-        <v>0.9714704193393734</v>
+        <v>0.9898927854180372</v>
       </c>
       <c r="F24">
-        <v>0.9854420345685541</v>
+        <v>0.9922843711096743</v>
       </c>
       <c r="G24">
-        <v>0.9854420345685537</v>
+        <v>0.9922843711096754</v>
       </c>
       <c r="H24">
-        <v>0.9854420345685537</v>
+        <v>0.9922843711096754</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D25">
-        <v>1.156507426534088</v>
+        <v>0.9312482317462356</v>
       </c>
       <c r="E25">
-        <v>1.156507426534088</v>
+        <v>0.9312482317462357</v>
       </c>
       <c r="F25">
-        <v>1.073863846931256</v>
+        <v>0.9602283340866721</v>
       </c>
       <c r="G25">
-        <v>1.073863846931255</v>
+        <v>0.9602283340866712</v>
       </c>
       <c r="H25">
-        <v>1.073863846931255</v>
+        <v>0.9602283340866712</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D26">
-        <v>1.327493129642546</v>
+        <v>0.8518766552821998</v>
       </c>
       <c r="E26">
-        <v>1.327493129642547</v>
+        <v>0.8518766552821998</v>
       </c>
       <c r="F26">
-        <v>1.151944994154603</v>
+        <v>0.9203297228677866</v>
       </c>
       <c r="G26">
-        <v>1.151944994154604</v>
+        <v>0.920329722867786</v>
       </c>
       <c r="H26">
-        <v>1.151944994154604</v>
+        <v>0.920329722867786</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D27">
-        <v>1.312036687250888</v>
+        <v>0.8258684171300312</v>
       </c>
       <c r="E27">
-        <v>1.312036687250888</v>
+        <v>0.8258684171300312</v>
       </c>
       <c r="F27">
-        <v>1.145413037702157</v>
+        <v>0.9060760259412903</v>
       </c>
       <c r="G27">
-        <v>1.145413037702156</v>
+        <v>0.9060760259412913</v>
       </c>
       <c r="H27">
-        <v>1.145413037702156</v>
+        <v>0.9060760259412913</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="A2:A27"/>
     <mergeCell ref="B2:B5"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="B16:B19"/>
     <mergeCell ref="B20:B23"/>
     <mergeCell ref="B24:B27"/>
   </mergeCells>
@@ -3277,10 +3250,10 @@
         <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>26</v>
@@ -3289,15 +3262,15 @@
         <v>22</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -3306,7 +3279,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E2">
         <v>0.9948291665814549</v>
@@ -3323,7 +3296,7 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E3">
         <v>54.44333246942244</v>
@@ -3340,7 +3313,7 @@
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E4">
         <v>0.9127929879518503</v>
@@ -3357,7 +3330,7 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E5">
         <v>1.624979345855552</v>
@@ -3374,7 +3347,7 @@
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E6">
         <v>1.23723084743343</v>
@@ -3393,7 +3366,7 @@
         <v>4</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E7">
         <v>0.9828690353622259</v>
@@ -3410,7 +3383,7 @@
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E8">
         <v>57.31648804859531</v>
@@ -3427,7 +3400,7 @@
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E9">
         <v>0.9611726444439505</v>
@@ -3444,7 +3417,7 @@
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E10">
         <v>1.241351879997542</v>
@@ -3461,7 +3434,7 @@
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E11">
         <v>1.075404496003537</v>
@@ -3480,7 +3453,7 @@
         <v>16</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E12">
         <v>1.001053300118882</v>
@@ -3497,7 +3470,7 @@
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E13">
         <v>43.42024113565012</v>
@@ -3514,7 +3487,7 @@
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E14">
         <v>1.410243318375383</v>
@@ -3531,7 +3504,7 @@
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E15">
         <v>0.8987783717152672</v>
@@ -3548,7 +3521,7 @@
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E16">
         <v>0.7646716010102846</v>
@@ -3567,7 +3540,7 @@
         <v>64</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E17">
         <v>1.027586485217014</v>
@@ -3584,7 +3557,7 @@
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E18">
         <v>1.822972891700415</v>
@@ -3601,7 +3574,7 @@
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E19">
         <v>0.1966315129912789</v>
@@ -3618,7 +3591,7 @@
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E20">
         <v>0.1423169151194792</v>
@@ -3635,7 +3608,7 @@
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E21">
         <v>0.1432773672588193</v>
@@ -3656,7 +3629,7 @@
         <v>1</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E22">
         <v>1.001536766781934</v>
@@ -3673,7 +3646,7 @@
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E23">
         <v>81.05855148114225</v>
@@ -3690,7 +3663,7 @@
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E24">
         <v>1.010299128954704</v>
@@ -3707,7 +3680,7 @@
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E25">
         <v>1.58944110655908</v>
@@ -3724,7 +3697,7 @@
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E26">
         <v>1.301204753422241</v>
@@ -3743,7 +3716,7 @@
         <v>4</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E27">
         <v>0.9981288126564584</v>
@@ -3760,7 +3733,7 @@
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E28">
         <v>58.17042970376627</v>
@@ -3777,7 +3750,7 @@
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E29">
         <v>0.8106548383531055</v>
@@ -3794,7 +3767,7 @@
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E30">
         <v>1.134406414693613</v>
@@ -3811,7 +3784,7 @@
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E31">
         <v>0.910233805551894</v>
@@ -3830,7 +3803,7 @@
         <v>16</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E32">
         <v>1.001253258669881</v>
@@ -3847,7 +3820,7 @@
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E33">
         <v>22.89421526758385</v>
@@ -3864,7 +3837,7 @@
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E34">
         <v>1.340669436901159</v>
@@ -3881,7 +3854,7 @@
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E35">
         <v>0.7712558113665313</v>
@@ -3898,7 +3871,7 @@
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E36">
         <v>0.7544986694911141</v>
@@ -3917,7 +3890,7 @@
         <v>64</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E37">
         <v>0.9961226373864465</v>
@@ -3934,7 +3907,7 @@
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E38">
         <v>4.86952931142739</v>
@@ -3951,7 +3924,7 @@
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E39">
         <v>0.3593577161683076</v>
@@ -3968,7 +3941,7 @@
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E40">
         <v>0.2565601018035494</v>
@@ -3985,7 +3958,7 @@
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E41">
         <v>0.270987714591887</v>
@@ -4006,7 +3979,7 @@
         <v>1</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E42">
         <v>1.00930600593982</v>
@@ -4023,7 +3996,7 @@
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E43">
         <v>58.47987121215872</v>
@@ -4040,7 +4013,7 @@
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E44">
         <v>0.8553978979504632</v>
@@ -4057,7 +4030,7 @@
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E45">
         <v>1.742400755461952</v>
@@ -4074,7 +4047,7 @@
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E46">
         <v>1.083071498189555</v>
@@ -4093,7 +4066,7 @@
         <v>4</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E47">
         <v>1.008417714346194</v>
@@ -4110,7 +4083,7 @@
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E48">
         <v>43.06293004600846</v>
@@ -4127,7 +4100,7 @@
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E49">
         <v>0.8511631820834727</v>
@@ -4144,7 +4117,7 @@
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E50">
         <v>1.202202916406758</v>
@@ -4161,7 +4134,7 @@
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E51">
         <v>0.9563674124576002</v>
@@ -4180,7 +4153,7 @@
         <v>16</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E52">
         <v>0.9975915678358964</v>
@@ -4197,7 +4170,7 @@
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E53">
         <v>17.19339710123357</v>
@@ -4214,7 +4187,7 @@
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E54">
         <v>0.6299090320942654</v>
@@ -4231,7 +4204,7 @@
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E55">
         <v>0.4629526287202225</v>
@@ -4248,7 +4221,7 @@
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E56">
         <v>0.4282358323092799</v>
@@ -4267,7 +4240,7 @@
         <v>64</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E57">
         <v>1.00101407378119</v>
@@ -4284,7 +4257,7 @@
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E58">
         <v>1.379550398437717</v>
@@ -4301,7 +4274,7 @@
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E59">
         <v>0.1434554299789456</v>
@@ -4318,7 +4291,7 @@
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E60">
         <v>0.1283954145031218</v>
@@ -4335,7 +4308,7 @@
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E61">
         <v>0.1312708327194214</v>
@@ -4356,7 +4329,7 @@
         <v>1</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E62">
         <v>1.000782848212709</v>
@@ -4373,7 +4346,7 @@
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E63">
         <v>62.57470493925121</v>
@@ -4390,7 +4363,7 @@
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E64">
         <v>0.8403164695812335</v>
@@ -4407,7 +4380,7 @@
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E65">
         <v>1.246730236683945</v>
@@ -4424,7 +4397,7 @@
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E66">
         <v>1.400856869801522</v>
@@ -4443,7 +4416,7 @@
         <v>4</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E67">
         <v>1.012617056079331</v>
@@ -4460,7 +4433,7 @@
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E68">
         <v>39.73548193003253</v>
@@ -4477,7 +4450,7 @@
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E69">
         <v>0.8767332663436763</v>
@@ -4494,7 +4467,7 @@
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E70">
         <v>1.310074180708307</v>
@@ -4511,7 +4484,7 @@
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
       <c r="D71" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E71">
         <v>1.064078056171657</v>
@@ -4530,7 +4503,7 @@
         <v>16</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E72">
         <v>0.9960749264626991</v>
@@ -4547,7 +4520,7 @@
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E73">
         <v>21.65442110502682</v>
@@ -4564,7 +4537,7 @@
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E74">
         <v>0.5601410243252849</v>
@@ -4581,7 +4554,7 @@
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E75">
         <v>0.4184787853373956</v>
@@ -4598,7 +4571,7 @@
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E76">
         <v>0.3892745828291316</v>
@@ -4617,7 +4590,7 @@
         <v>64</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E77">
         <v>1.00239561256814</v>
@@ -4634,7 +4607,7 @@
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
       <c r="D78" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E78">
         <v>1.127501975919327</v>
@@ -4651,7 +4624,7 @@
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
       <c r="D79" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E79">
         <v>0.1308789128796715</v>
@@ -4668,7 +4641,7 @@
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E80">
         <v>0.1188315741537491</v>
@@ -4685,7 +4658,7 @@
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
       <c r="D81" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E81">
         <v>0.139459747334728</v>
@@ -4706,7 +4679,7 @@
         <v>1</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E82">
         <v>0.987588072491096</v>
@@ -4723,7 +4696,7 @@
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
       <c r="D83" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E83">
         <v>26.46800417606596</v>
@@ -4740,7 +4713,7 @@
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
       <c r="D84" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E84">
         <v>0.4032125219116118</v>
@@ -4757,7 +4730,7 @@
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
       <c r="D85" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E85">
         <v>0.5111569906391964</v>
@@ -4774,7 +4747,7 @@
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
       <c r="D86" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E86">
         <v>0.4512154441195955</v>
@@ -4793,7 +4766,7 @@
         <v>4</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E87">
         <v>0.9852291707080686</v>
@@ -4810,7 +4783,7 @@
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
       <c r="D88" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E88">
         <v>2.971429425638668</v>
@@ -4827,7 +4800,7 @@
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
       <c r="D89" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E89">
         <v>0.05966902483092803</v>
@@ -4844,7 +4817,7 @@
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
       <c r="D90" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E90">
         <v>0.06522356589325203</v>
@@ -4861,7 +4834,7 @@
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
       <c r="D91" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E91">
         <v>0.05512951935555748</v>
@@ -4880,7 +4853,7 @@
         <v>16</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E92">
         <v>0.9832020679359453</v>
@@ -4897,7 +4870,7 @@
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
       <c r="D93" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E93">
         <v>1.019618371794516</v>
@@ -4914,7 +4887,7 @@
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
       <c r="D94" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E94">
         <v>0.03942458479204555</v>
@@ -4931,7 +4904,7 @@
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
       <c r="D95" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E95">
         <v>0.03655953822700053</v>
@@ -4948,7 +4921,7 @@
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
       <c r="D96" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E96">
         <v>0.03504895991956235</v>
@@ -4967,7 +4940,7 @@
         <v>64</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E97">
         <v>1.107886123658194</v>
@@ -4984,7 +4957,7 @@
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
       <c r="D98" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E98">
         <v>3.06805946605373</v>
@@ -5001,7 +4974,7 @@
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
       <c r="D99" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E99">
         <v>0.4162004784423449</v>
@@ -5018,7 +4991,7 @@
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
       <c r="D100" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E100">
         <v>0.3061466954993906</v>
@@ -5035,7 +5008,7 @@
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
       <c r="D101" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E101">
         <v>0.3309462494374554</v>
@@ -5056,7 +5029,7 @@
         <v>1</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E102">
         <v>0.9728761783585753</v>
@@ -5073,7 +5046,7 @@
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
       <c r="D103" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E103">
         <v>1.02829562130818</v>
@@ -5090,7 +5063,7 @@
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
       <c r="D104" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E104">
         <v>0.01491917442158329</v>
@@ -5107,7 +5080,7 @@
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
       <c r="D105" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E105">
         <v>0.02224912797274432</v>
@@ -5124,7 +5097,7 @@
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
       <c r="D106" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E106">
         <v>0.02082948881314538</v>
@@ -5143,7 +5116,7 @@
         <v>4</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E107">
         <v>1.043522503783751</v>
@@ -5160,7 +5133,7 @@
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
       <c r="D108" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E108">
         <v>0.7090190667812396</v>
@@ -5177,7 +5150,7 @@
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
       <c r="D109" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E109">
         <v>0.01422236303458232</v>
@@ -5194,7 +5167,7 @@
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
       <c r="D110" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E110">
         <v>0.02422233956192955</v>
@@ -5211,7 +5184,7 @@
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
       <c r="D111" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E111">
         <v>0.0343931111021373</v>
@@ -5230,7 +5203,7 @@
         <v>16</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E112">
         <v>1.018452819192909</v>
@@ -5247,7 +5220,7 @@
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
       <c r="D113" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E113">
         <v>0.9249846523180282</v>
@@ -5264,7 +5237,7 @@
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
       <c r="D114" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E114">
         <v>0.06210216622770236</v>
@@ -5281,7 +5254,7 @@
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
       <c r="D115" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E115">
         <v>0.05799501613422537</v>
@@ -5298,7 +5271,7 @@
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
       <c r="D116" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E116">
         <v>0.06039955930350182</v>
@@ -5317,7 +5290,7 @@
         <v>64</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E117">
         <v>1.216292584280295</v>
@@ -5334,7 +5307,7 @@
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
       <c r="D118" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E118">
         <v>3.562908360474474</v>
@@ -5351,7 +5324,7 @@
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
       <c r="D119" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E119">
         <v>0.5802014644419288</v>
@@ -5368,7 +5341,7 @@
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
       <c r="D120" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E120">
         <v>0.3920418119090428</v>
@@ -5385,7 +5358,7 @@
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
       <c r="D121" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E121">
         <v>0.3541198214321543</v>

</xml_diff>